<commit_message>
Not making much progress
</commit_message>
<xml_diff>
--- a/CH-060 Match payments.xlsx
+++ b/CH-060 Match payments.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFCCA18B-5512-44D1-AB16-58936B509250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34377BE-68C2-401C-82E5-331BFF6C6DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="EDA" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$B$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$B$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$B$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="26">
   <si>
     <t>Result</t>
   </si>
@@ -114,6 +116,9 @@
   </si>
   <si>
     <t>Question Table 1 Recipts</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/feed/update/urn:li:activity:7202051165499396096?commentUrn=urn%3Ali%3Acomment%3A%28activity%3A7202051165499396096%2C7202085999735156737%29&amp;dashCommentUrn=urn%3Ali%3Afsd_comment%3A%287202085999735156737%2Curn%3Ali%3Aactivity%3A7202051165499396096%29</t>
   </si>
 </sst>
 </file>
@@ -1165,10 +1170,632 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:R74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" style="3" customWidth="1"/>
+    <col min="2" max="2" width="4.09765625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="12.19921875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="6.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.59765625" style="3"/>
+    <col min="6" max="6" width="4.19921875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.8984375" style="3" customWidth="1"/>
+    <col min="9" max="10" width="8.59765625" style="3"/>
+    <col min="11" max="16" width="6" style="3" customWidth="1"/>
+    <col min="17" max="16384" width="8.59765625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:18" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="F1" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="K1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="R1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="7"/>
+      <c r="L2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="10">
+        <v>45325</v>
+      </c>
+      <c r="D3" s="29">
+        <v>120</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="12">
+        <v>45278</v>
+      </c>
+      <c r="H3" s="31">
+        <v>600</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="33">
+        <v>120</v>
+      </c>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="15"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="16">
+        <v>45338</v>
+      </c>
+      <c r="D4" s="30">
+        <v>356</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="12">
+        <v>45286</v>
+      </c>
+      <c r="H4" s="31">
+        <v>50</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="33">
+        <v>356</v>
+      </c>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="34"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="16">
+        <v>45341</v>
+      </c>
+      <c r="D5" s="30">
+        <v>312</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="12">
+        <v>45312</v>
+      </c>
+      <c r="H5" s="31">
+        <v>112</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="33">
+        <v>124</v>
+      </c>
+      <c r="M5" s="33">
+        <v>50</v>
+      </c>
+      <c r="N5" s="33">
+        <v>112</v>
+      </c>
+      <c r="O5" s="33">
+        <v>26</v>
+      </c>
+      <c r="P5" s="34"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="16">
+        <v>45355</v>
+      </c>
+      <c r="D6" s="30">
+        <v>437</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="12">
+        <v>45315</v>
+      </c>
+      <c r="H6" s="31">
+        <v>800</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33">
+        <v>437</v>
+      </c>
+      <c r="P6" s="34"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="16">
+        <v>45364</v>
+      </c>
+      <c r="D7" s="30">
+        <v>374</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="19">
+        <v>45327</v>
+      </c>
+      <c r="H7" s="32">
+        <v>1800</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33">
+        <v>337</v>
+      </c>
+      <c r="P7" s="34">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="16">
+        <v>45365</v>
+      </c>
+      <c r="D8" s="30">
+        <v>258</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="34">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="16">
+        <v>45370</v>
+      </c>
+      <c r="D9" s="30">
+        <v>369</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="17"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="34">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="16">
+        <v>45376</v>
+      </c>
+      <c r="D10" s="30">
+        <v>418</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="17"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="34">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="16">
+        <v>45384</v>
+      </c>
+      <c r="D11" s="30">
+        <v>308</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="17"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="34">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="16">
+        <v>45397</v>
+      </c>
+      <c r="D12" s="30">
+        <v>410</v>
+      </c>
+      <c r="G12" s="20"/>
+      <c r="K12" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="17"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="34">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="16">
+        <v>45406</v>
+      </c>
+      <c r="D13" s="30">
+        <v>491</v>
+      </c>
+      <c r="G13" s="20"/>
+      <c r="K13" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="P13" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="16">
+        <v>45409</v>
+      </c>
+      <c r="D14" s="30">
+        <v>50</v>
+      </c>
+      <c r="G14" s="20"/>
+      <c r="K14" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="O14" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="P14" s="26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="G15" s="20"/>
+      <c r="L15" s="27"/>
+      <c r="O15" s="20"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="G16" s="20"/>
+      <c r="L16" s="27"/>
+      <c r="O16" s="20"/>
+    </row>
+    <row r="17" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G17" s="20"/>
+      <c r="L17" s="27"/>
+      <c r="O17" s="20"/>
+    </row>
+    <row r="18" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G18" s="20"/>
+      <c r="L18" s="27"/>
+      <c r="O18" s="20"/>
+    </row>
+    <row r="19" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="L19" s="20"/>
+      <c r="O19" s="20"/>
+    </row>
+    <row r="20" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="L20" s="20"/>
+      <c r="O20" s="20"/>
+    </row>
+    <row r="21" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="L21" s="20"/>
+      <c r="O21" s="20"/>
+    </row>
+    <row r="22" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="L22" s="20"/>
+      <c r="O22" s="20"/>
+    </row>
+    <row r="23" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="L23" s="20"/>
+      <c r="O23" s="20"/>
+    </row>
+    <row r="24" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="L24" s="20"/>
+      <c r="O24" s="20"/>
+    </row>
+    <row r="25" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="L25" s="20"/>
+      <c r="O25" s="20"/>
+    </row>
+    <row r="26" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="L26" s="20"/>
+      <c r="O26" s="20"/>
+    </row>
+    <row r="27" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="L27" s="20"/>
+      <c r="O27" s="20"/>
+    </row>
+    <row r="28" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="L28" s="20"/>
+      <c r="O28" s="20"/>
+    </row>
+    <row r="29" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="O29" s="20"/>
+    </row>
+    <row r="30" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="O30" s="20"/>
+    </row>
+    <row r="31" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="O31" s="20"/>
+    </row>
+    <row r="32" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="O32" s="20"/>
+    </row>
+    <row r="33" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O33" s="20"/>
+    </row>
+    <row r="34" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O34" s="20"/>
+    </row>
+    <row r="35" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O35" s="20"/>
+    </row>
+    <row r="36" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O36" s="20"/>
+    </row>
+    <row r="37" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O37" s="20"/>
+    </row>
+    <row r="38" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O38" s="20"/>
+    </row>
+    <row r="39" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O39" s="20"/>
+    </row>
+    <row r="40" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O40" s="20"/>
+    </row>
+    <row r="41" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O41" s="20"/>
+    </row>
+    <row r="42" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O42" s="20"/>
+    </row>
+    <row r="43" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O43" s="20"/>
+    </row>
+    <row r="44" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O44" s="20"/>
+    </row>
+    <row r="45" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O45" s="20"/>
+    </row>
+    <row r="46" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O46" s="20"/>
+    </row>
+    <row r="47" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O47" s="20"/>
+    </row>
+    <row r="48" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O48" s="20"/>
+    </row>
+    <row r="49" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O49" s="20"/>
+    </row>
+    <row r="50" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O50" s="20"/>
+    </row>
+    <row r="51" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O51" s="20"/>
+    </row>
+    <row r="52" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O52" s="20"/>
+    </row>
+    <row r="53" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O53" s="20"/>
+    </row>
+    <row r="54" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O54" s="20"/>
+    </row>
+    <row r="55" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O55" s="20"/>
+    </row>
+    <row r="56" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O56" s="20"/>
+    </row>
+    <row r="57" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O57" s="20"/>
+    </row>
+    <row r="58" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O58" s="20"/>
+    </row>
+    <row r="59" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O59" s="20"/>
+    </row>
+    <row r="60" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O60" s="20"/>
+    </row>
+    <row r="61" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O61" s="20"/>
+    </row>
+    <row r="62" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O62" s="20"/>
+    </row>
+    <row r="63" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O63" s="20"/>
+    </row>
+    <row r="64" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O64" s="20"/>
+    </row>
+    <row r="65" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O65" s="20"/>
+    </row>
+    <row r="66" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O66" s="20"/>
+    </row>
+    <row r="67" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O67" s="20"/>
+    </row>
+    <row r="68" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O68" s="20"/>
+    </row>
+    <row r="69" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O69" s="20"/>
+    </row>
+    <row r="70" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O70" s="20"/>
+    </row>
+    <row r="71" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O71" s="20"/>
+    </row>
+    <row r="72" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O72" s="20"/>
+    </row>
+    <row r="73" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O73" s="20"/>
+    </row>
+    <row r="74" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O74" s="20"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G12:G16">
+    <sortCondition ref="G12:G16"/>
+  </sortState>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="K1:P1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62F3CE8-EB31-4D8F-AAFD-E96DF7E64363}">
   <dimension ref="B1:P74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1767,17 +2394,12 @@
       <c r="O74" s="20"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G12:G16">
-    <sortCondition ref="G12:G16"/>
-  </sortState>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="K1:P1"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
I understand the problem better
</commit_message>
<xml_diff>
--- a/CH-060 Match payments.xlsx
+++ b/CH-060 Match payments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BA6FAD-5662-4BE1-AB77-AE8031F83B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D80A31-40BF-4AC6-BF38-A1F74E855394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="26">
   <si>
     <t>Result</t>
   </si>
@@ -161,7 +161,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +197,14 @@
       <name val="Century Gothic"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -415,10 +423,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -512,17 +521,22 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -550,8 +564,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>565150</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -566,8 +580,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2152650" y="1517650"/>
-          <a:ext cx="3657600" cy="2235200"/>
+          <a:off x="2143760" y="1540510"/>
+          <a:ext cx="3641090" cy="2879090"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -1826,7 +1840,7 @@
   <dimension ref="B1:R74"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+      <selection activeCell="S5" sqref="S5:S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1845,24 +1859,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="F1" s="35" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="F1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="K1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="K1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
       <c r="R1" s="1" t="s">
         <v>25</v>
       </c>
@@ -2445,10 +2459,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62F3CE8-EB31-4D8F-AAFD-E96DF7E64363}">
-  <dimension ref="B1:P74"/>
+  <dimension ref="B1:X74"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="C14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2458,7 +2472,7 @@
     <col min="3" max="3" width="12.19921875" style="28" customWidth="1"/>
     <col min="4" max="4" width="6.5" style="3" customWidth="1"/>
     <col min="5" max="5" width="8.59765625" style="3"/>
-    <col min="6" max="6" width="4.19921875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.796875" style="3" customWidth="1"/>
     <col min="7" max="7" width="10.3984375" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.8984375" style="3" customWidth="1"/>
     <col min="9" max="10" width="8.59765625" style="3"/>
@@ -2467,24 +2481,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="F1" s="35" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="F1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="K1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="K1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -2858,66 +2872,716 @@
       <c r="L16" s="27"/>
       <c r="O16" s="20"/>
     </row>
-    <row r="17" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
       <c r="G17" s="20"/>
       <c r="L17" s="27"/>
       <c r="O17" s="20"/>
     </row>
-    <row r="18" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
       <c r="G18" s="20"/>
       <c r="L18" s="27"/>
       <c r="O18" s="20"/>
     </row>
-    <row r="19" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B19" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="10">
+        <v>45325</v>
+      </c>
+      <c r="D19" s="29">
+        <v>120</v>
+      </c>
+      <c r="E19" s="3">
+        <f>SUMIF($G$3:$G$7,"&lt;="&amp;C19,$H$3:$H$7)</f>
+        <v>1562</v>
+      </c>
+      <c r="F19" s="38">
+        <f>SUM($D$19:D19)</f>
+        <v>120</v>
+      </c>
+      <c r="G19" s="3" t="e">
+        <f>_xlfn.XLOOKUP(F19,$J$19:$J$23,$I$19:$I$23,,-1)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" s="38">
+        <f>SUM($H$3:H3)</f>
+        <v>600</v>
+      </c>
       <c r="L19" s="20"/>
-      <c r="O19" s="20"/>
-    </row>
-    <row r="20" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="N19" s="3" cm="1">
+        <f t="array" ref="N19:R30">_xlfn.LET(
+_xlpm.s,_xlfn.SEQUENCE(5),
+_xlpm.i,_xlfn.CHOOSECOLS(_xlfn.REDUCE(D3:D14,
+                    H3:H7,
+                    _xlfn.LAMBDA(_xlpm.a,_xlpm.w,_xlfn.LET(_xlpm.v,_xlfn.TAKE(_xlpm.a,,-1),
+                                          _xlpm.e,_xlfn.DROP(_xlfn.SCAN(,_xlfn.VSTACK(_xlpm.w,_xlpm.v),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlpm.a-_xlpm.v)),-1),
+_xlfn.HSTACK(_xlpm.a,_xlfn.IFS(_xlpm.e&gt;_xlpm.v,_xlpm.v,_xlpm.e&gt;0,_xlpm.e,1,),_xlfn.IFS(_xlpm.e&gt;_xlpm.v,0,_xlpm.e&lt;0,_xlpm.v,1,_xlpm.v-_xlpm.e))))),_xlpm.s*2),IF(MMULT(_xlpm.i,_xlpm.s^0),_xlpm.i,"NP"))</f>
+        <v>120</v>
+      </c>
+      <c r="O19" s="20">
+        <v>0</v>
+      </c>
+      <c r="P19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>0</v>
+      </c>
+      <c r="R19" s="3">
+        <v>0</v>
+      </c>
+      <c r="T19" s="3" cm="1">
+        <f t="array" ref="T19:X30">_xlfn.LET(
+_xlpm.s,_xlfn.SEQUENCE(5),
+_xlpm.i,_xlfn.CHOOSECOLS(_xlfn.REDUCE(D3:D14,
+                    H3:H7,
+                    _xlfn.LAMBDA(_xlpm.a,_xlpm.w,_xlfn.LET(_xlpm.v,_xlfn.TAKE(_xlpm.a,,-1),
+                                          _xlpm.e,_xlfn.DROP(_xlfn.SCAN(,_xlfn.VSTACK(_xlpm.w,_xlpm.v),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlpm.a-_xlpm.v)),-1),
+                     _xlfn.HSTACK(_xlpm.a,_xlfn.IFS(_xlpm.e&gt;_xlpm.v,_xlpm.v,_xlpm.e&gt;0,_xlpm.e,1,),_xlfn.IFS(_xlpm.e&gt;_xlpm.v,0,_xlpm.e&lt;0,_xlpm.v,1,_xlpm.v-_xlpm.e))))),_xlpm.s*2),
+_xlpm.i)</f>
+        <v>120</v>
+      </c>
+      <c r="U19" s="3">
+        <v>0</v>
+      </c>
+      <c r="V19" s="3">
+        <v>0</v>
+      </c>
+      <c r="W19" s="3">
+        <v>0</v>
+      </c>
+      <c r="X19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B20" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="16">
+        <v>45338</v>
+      </c>
+      <c r="D20" s="30">
+        <v>356</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" ref="E20:E30" si="0">SUMIF($G$3:$G$7,"&lt;="&amp;C20,$H$3:$H$7)</f>
+        <v>3362</v>
+      </c>
+      <c r="F20" s="38">
+        <f>SUM($D$19:D20)</f>
+        <v>476</v>
+      </c>
+      <c r="G20" s="3" t="e">
+        <f t="shared" ref="G20:G30" si="1">_xlfn.XLOOKUP(F20,$J$19:$J$23,$I$19:$I$23,,-1)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="38">
+        <f>SUM($H$3:H4)</f>
+        <v>650</v>
+      </c>
       <c r="L20" s="20"/>
-      <c r="O20" s="20"/>
-    </row>
-    <row r="21" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="N20" s="3">
+        <v>356</v>
+      </c>
+      <c r="O20" s="20">
+        <v>0</v>
+      </c>
+      <c r="P20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>0</v>
+      </c>
+      <c r="R20" s="3">
+        <v>0</v>
+      </c>
+      <c r="T20" s="3">
+        <v>356</v>
+      </c>
+      <c r="U20" s="3">
+        <v>0</v>
+      </c>
+      <c r="V20" s="3">
+        <v>0</v>
+      </c>
+      <c r="W20" s="3">
+        <v>0</v>
+      </c>
+      <c r="X20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="16">
+        <v>45341</v>
+      </c>
+      <c r="D21" s="30">
+        <v>312</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="0"/>
+        <v>3362</v>
+      </c>
+      <c r="F21" s="38">
+        <f>SUM($D$19:D21)</f>
+        <v>788</v>
+      </c>
+      <c r="G21" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>P3</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="38">
+        <f>SUM($H$3:H5)</f>
+        <v>762</v>
+      </c>
       <c r="L21" s="20"/>
-      <c r="O21" s="20"/>
-    </row>
-    <row r="22" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="N21" s="3">
+        <v>124</v>
+      </c>
+      <c r="O21" s="20">
+        <v>50</v>
+      </c>
+      <c r="P21" s="3">
+        <v>112</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>26</v>
+      </c>
+      <c r="R21" s="3">
+        <v>0</v>
+      </c>
+      <c r="T21" s="3">
+        <v>124</v>
+      </c>
+      <c r="U21" s="3">
+        <v>50</v>
+      </c>
+      <c r="V21" s="3">
+        <v>112</v>
+      </c>
+      <c r="W21" s="3">
+        <v>26</v>
+      </c>
+      <c r="X21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="16">
+        <v>45355</v>
+      </c>
+      <c r="D22" s="30">
+        <v>437</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="0"/>
+        <v>3362</v>
+      </c>
+      <c r="F22" s="38">
+        <f>SUM($D$19:D22)</f>
+        <v>1225</v>
+      </c>
+      <c r="G22" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>P3</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="38">
+        <f>SUM($H$3:H6)</f>
+        <v>1562</v>
+      </c>
       <c r="L22" s="20"/>
-      <c r="O22" s="20"/>
-    </row>
-    <row r="23" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="N22" s="3">
+        <v>0</v>
+      </c>
+      <c r="O22" s="20">
+        <v>0</v>
+      </c>
+      <c r="P22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>437</v>
+      </c>
+      <c r="R22" s="3">
+        <v>0</v>
+      </c>
+      <c r="T22" s="3">
+        <v>0</v>
+      </c>
+      <c r="U22" s="3">
+        <v>0</v>
+      </c>
+      <c r="V22" s="3">
+        <v>0</v>
+      </c>
+      <c r="W22" s="3">
+        <v>437</v>
+      </c>
+      <c r="X22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="16">
+        <v>45364</v>
+      </c>
+      <c r="D23" s="30">
+        <v>374</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="0"/>
+        <v>3362</v>
+      </c>
+      <c r="F23" s="38">
+        <f>SUM($D$19:D23)</f>
+        <v>1599</v>
+      </c>
+      <c r="G23" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>P4</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="38">
+        <f>SUM($H$3:H7)</f>
+        <v>3362</v>
+      </c>
       <c r="L23" s="20"/>
-      <c r="O23" s="20"/>
-    </row>
-    <row r="24" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="N23" s="3">
+        <v>0</v>
+      </c>
+      <c r="O23" s="20">
+        <v>0</v>
+      </c>
+      <c r="P23" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>337</v>
+      </c>
+      <c r="R23" s="3">
+        <v>37</v>
+      </c>
+      <c r="T23" s="3">
+        <v>0</v>
+      </c>
+      <c r="U23" s="3">
+        <v>0</v>
+      </c>
+      <c r="V23" s="3">
+        <v>0</v>
+      </c>
+      <c r="W23" s="3">
+        <v>337</v>
+      </c>
+      <c r="X23" s="3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="16">
+        <v>45365</v>
+      </c>
+      <c r="D24" s="30">
+        <v>258</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>3362</v>
+      </c>
+      <c r="F24" s="38">
+        <f>SUM($D$19:D24)</f>
+        <v>1857</v>
+      </c>
+      <c r="G24" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>P4</v>
+      </c>
       <c r="L24" s="20"/>
-      <c r="O24" s="20"/>
-    </row>
-    <row r="25" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="N24" s="3">
+        <v>0</v>
+      </c>
+      <c r="O24" s="20">
+        <v>0</v>
+      </c>
+      <c r="P24" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>0</v>
+      </c>
+      <c r="R24" s="3">
+        <v>258</v>
+      </c>
+      <c r="T24" s="3">
+        <v>0</v>
+      </c>
+      <c r="U24" s="3">
+        <v>0</v>
+      </c>
+      <c r="V24" s="3">
+        <v>0</v>
+      </c>
+      <c r="W24" s="3">
+        <v>0</v>
+      </c>
+      <c r="X24" s="3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="16">
+        <v>45370</v>
+      </c>
+      <c r="D25" s="30">
+        <v>369</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>3362</v>
+      </c>
+      <c r="F25" s="38">
+        <f>SUM($D$19:D25)</f>
+        <v>2226</v>
+      </c>
+      <c r="G25" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>P4</v>
+      </c>
       <c r="L25" s="20"/>
-      <c r="O25" s="20"/>
-    </row>
-    <row r="26" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="N25" s="3">
+        <v>0</v>
+      </c>
+      <c r="O25" s="20">
+        <v>0</v>
+      </c>
+      <c r="P25" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>0</v>
+      </c>
+      <c r="R25" s="3">
+        <v>369</v>
+      </c>
+      <c r="T25" s="3">
+        <v>0</v>
+      </c>
+      <c r="U25" s="3">
+        <v>0</v>
+      </c>
+      <c r="V25" s="3">
+        <v>0</v>
+      </c>
+      <c r="W25" s="3">
+        <v>0</v>
+      </c>
+      <c r="X25" s="3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="16">
+        <v>45376</v>
+      </c>
+      <c r="D26" s="30">
+        <v>418</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="0"/>
+        <v>3362</v>
+      </c>
+      <c r="F26" s="38">
+        <f>SUM($D$19:D26)</f>
+        <v>2644</v>
+      </c>
+      <c r="G26" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>P4</v>
+      </c>
       <c r="L26" s="20"/>
-      <c r="O26" s="20"/>
-    </row>
-    <row r="27" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="N26" s="3">
+        <v>0</v>
+      </c>
+      <c r="O26" s="20">
+        <v>0</v>
+      </c>
+      <c r="P26" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>0</v>
+      </c>
+      <c r="R26" s="3">
+        <v>418</v>
+      </c>
+      <c r="T26" s="3">
+        <v>0</v>
+      </c>
+      <c r="U26" s="3">
+        <v>0</v>
+      </c>
+      <c r="V26" s="3">
+        <v>0</v>
+      </c>
+      <c r="W26" s="3">
+        <v>0</v>
+      </c>
+      <c r="X26" s="3">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="16">
+        <v>45384</v>
+      </c>
+      <c r="D27" s="30">
+        <v>308</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="0"/>
+        <v>3362</v>
+      </c>
+      <c r="F27" s="38">
+        <f>SUM($D$19:D27)</f>
+        <v>2952</v>
+      </c>
+      <c r="G27" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>P4</v>
+      </c>
       <c r="L27" s="20"/>
-      <c r="O27" s="20"/>
-    </row>
-    <row r="28" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="N27" s="3">
+        <v>0</v>
+      </c>
+      <c r="O27" s="20">
+        <v>0</v>
+      </c>
+      <c r="P27" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>0</v>
+      </c>
+      <c r="R27" s="3">
+        <v>308</v>
+      </c>
+      <c r="T27" s="3">
+        <v>0</v>
+      </c>
+      <c r="U27" s="3">
+        <v>0</v>
+      </c>
+      <c r="V27" s="3">
+        <v>0</v>
+      </c>
+      <c r="W27" s="3">
+        <v>0</v>
+      </c>
+      <c r="X27" s="3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B28" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="16">
+        <v>45397</v>
+      </c>
+      <c r="D28" s="30">
+        <v>410</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="0"/>
+        <v>3362</v>
+      </c>
+      <c r="F28" s="38">
+        <f>SUM($D$19:D28)</f>
+        <v>3362</v>
+      </c>
+      <c r="G28" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>P5</v>
+      </c>
       <c r="L28" s="20"/>
-      <c r="O28" s="20"/>
-    </row>
-    <row r="29" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="O29" s="20"/>
-    </row>
-    <row r="30" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="O30" s="20"/>
-    </row>
-    <row r="31" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="N28" s="3">
+        <v>0</v>
+      </c>
+      <c r="O28" s="20">
+        <v>0</v>
+      </c>
+      <c r="P28" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>0</v>
+      </c>
+      <c r="R28" s="3">
+        <v>410</v>
+      </c>
+      <c r="T28" s="3">
+        <v>0</v>
+      </c>
+      <c r="U28" s="3">
+        <v>0</v>
+      </c>
+      <c r="V28" s="3">
+        <v>0</v>
+      </c>
+      <c r="W28" s="3">
+        <v>0</v>
+      </c>
+      <c r="X28" s="3">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B29" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="16">
+        <v>45406</v>
+      </c>
+      <c r="D29" s="30">
+        <v>491</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="0"/>
+        <v>3362</v>
+      </c>
+      <c r="F29" s="38">
+        <f>SUM($D$19:D29)</f>
+        <v>3853</v>
+      </c>
+      <c r="G29" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>P5</v>
+      </c>
+      <c r="N29" s="3" t="str">
+        <v>NP</v>
+      </c>
+      <c r="O29" s="20" t="str">
+        <v>NP</v>
+      </c>
+      <c r="P29" s="3" t="str">
+        <v>NP</v>
+      </c>
+      <c r="Q29" s="3" t="str">
+        <v>NP</v>
+      </c>
+      <c r="R29" s="3" t="str">
+        <v>NP</v>
+      </c>
+      <c r="T29" s="3">
+        <v>0</v>
+      </c>
+      <c r="U29" s="3">
+        <v>0</v>
+      </c>
+      <c r="V29" s="3">
+        <v>0</v>
+      </c>
+      <c r="W29" s="3">
+        <v>0</v>
+      </c>
+      <c r="X29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B30" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="16">
+        <v>45409</v>
+      </c>
+      <c r="D30" s="30">
+        <v>50</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="0"/>
+        <v>3362</v>
+      </c>
+      <c r="F30" s="38">
+        <f>SUM($D$19:D30)</f>
+        <v>3903</v>
+      </c>
+      <c r="G30" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>P5</v>
+      </c>
+      <c r="N30" s="3" t="str">
+        <v>NP</v>
+      </c>
+      <c r="O30" s="20" t="str">
+        <v>NP</v>
+      </c>
+      <c r="P30" s="3" t="str">
+        <v>NP</v>
+      </c>
+      <c r="Q30" s="3" t="str">
+        <v>NP</v>
+      </c>
+      <c r="R30" s="3" t="str">
+        <v>NP</v>
+      </c>
+      <c r="T30" s="3">
+        <v>0</v>
+      </c>
+      <c r="U30" s="3">
+        <v>0</v>
+      </c>
+      <c r="V30" s="3">
+        <v>0</v>
+      </c>
+      <c r="W30" s="3">
+        <v>0</v>
+      </c>
+      <c r="X30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
       <c r="O31" s="20"/>
     </row>
-    <row r="32" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
       <c r="O32" s="20"/>
     </row>
     <row r="33" spans="15:15" x14ac:dyDescent="0.25">
@@ -3061,17 +3725,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E485CBBF-769F-44F4-83CF-110C31EDB775}">
   <dimension ref="B1:R74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="3" customWidth="1"/>
     <col min="2" max="2" width="4.3984375" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.8984375" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.8984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="4.8984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.19921875" style="3" customWidth="1"/>
+    <col min="5" max="6" width="4.8984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.19921875" style="3" customWidth="1"/>
     <col min="8" max="8" width="10.8984375" style="3" customWidth="1"/>
     <col min="9" max="10" width="8.59765625" style="3"/>
     <col min="11" max="11" width="6" style="3" customWidth="1"/>
@@ -3081,25 +3746,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="F1" s="35" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="F1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="K1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="R1" s="1" t="s">
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="K1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="R1" s="39" t="s">
         <v>25</v>
       </c>
     </row>
@@ -4159,8 +4824,11 @@
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="K1:P1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="R1" r:id="rId1" display="https://www.linkedin.com/feed/update/urn:li:activity:7202051165499396096?commentUrn=urn%3Ali%3Acomment%3A%28activity%3A7202051165499396096%2C7202085999735156737%29&amp;dashCommentUrn=urn%3Ali%3Afsd_comment%3A%287202085999735156737%2Curn%3Ali%3Aactivity%3A7202051165499396096%29" xr:uid="{3997F4B3-0867-4454-82F8-3535C33A6AE8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4168,7 +4836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D4DF196-8AFA-4D1D-A7A2-D917C2856F88}">
   <dimension ref="B1:Q74"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -4188,24 +4856,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="F1" s="35" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="F1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="K1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="K1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -4585,7 +5253,7 @@
       <c r="O17" s="20"/>
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C18" s="37"/>
+      <c r="C18" s="35"/>
       <c r="G18" s="20"/>
       <c r="L18" s="27"/>
       <c r="O18" s="20"/>

</xml_diff>

<commit_message>
Finally got Bo's solution to work
</commit_message>
<xml_diff>
--- a/CH-060 Match payments.xlsx
+++ b/CH-060 Match payments.xlsx
@@ -8,22 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D80A31-40BF-4AC6-BF38-A1F74E855394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F2A04B-9714-4D45-98FC-353F0A4FF428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alternate" sheetId="3" r:id="rId3"/>
     <sheet name="Alternate2" sheetId="4" r:id="rId4"/>
+    <sheet name="Alternate3" sheetId="5" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Alternate!$B$2:$B$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Alternate2!$B$2:$B$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Alternate3!$B$2:$B$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$B$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$B$15</definedName>
     <definedName name="allocate_payment">_xlfn.LAMBDA(_xlpm.costs,_xlpm.payments,_xlpm.allocations,_xlpm.position, _xlfn.LET(_xlpm._costRows, ROWS(_xlpm.costs), _xlpm._paymentColumns, COLUMNS(_xlpm.payments), _xlpm._seq, _xlfn.WRAPCOLS(_xlfn.SEQUENCE(_xlpm._costRows * _xlpm._paymentColumns), _xlpm._costRows), _xlpm._col, INT((_xlpm.position - 1) / _xlpm._costRows) + 1, _xlpm._row, MOD(_xlpm.position - 1, _xlpm._costRows) + 1, _xlpm._cost, INDEX(_xlpm.costs, _xlpm._row, 1), _xlpm._payment, INDEX(_xlpm.payments, 1, _xlpm._col), _xlpm._newAllocation, IF(_xlpm._cost &lt;= _xlpm._payment, _xlpm._cost, _xlpm._payment), _xlpm._newAllocations, IF(_xlpm._seq = _xlpm.position, _xlpm._newAllocation, 0) + _xlpm.allocations, _xlpm._newTotal, _xlfn.LAMBDA(_xlpm.seq,_xlpm.pos,_xlpm.arr, IF(_xlpm.seq = _xlpm.pos, _xlpm.arr - _xlpm._newAllocation, _xlpm.arr)), _xlpm._newCosts, _xlpm._newTotal(_xlfn.SEQUENCE(_xlpm._costRows), _xlpm._row, _xlpm.costs), _xlpm._newPayments, _xlpm._newTotal(_xlfn.SEQUENCE(, _xlpm._paymentColumns), _xlpm._col, _xlpm.payments), IF((_xlpm.position + 1) &gt; MAX(_xlpm._seq), _xlpm._newAllocations, allocate_payment(_xlpm._newCosts, _xlpm._newPayments, _xlpm._newAllocations, _xlpm.position + 1))))</definedName>
@@ -74,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="27">
   <si>
     <t>Result</t>
   </si>
@@ -152,6 +154,9 @@
   </si>
   <si>
     <t>https://www.linkedin.com/feed/update/urn:li:activity:7202051165499396096?commentUrn=urn%3Ali%3Acomment%3A%28activity%3A7202051165499396096%2C7202085999735156737%29&amp;dashCommentUrn=urn%3Ali%3Afsd_comment%3A%287202085999735156737%2Curn%3Ali%3Aactivity%3A7202051165499396096%29</t>
+  </si>
+  <si>
+    <t>I found the issue. Some problem with my Excel version.</t>
   </si>
 </sst>
 </file>
@@ -427,7 +432,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -524,15 +529,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1805,7 +1814,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="958" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="715" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1859,24 +1868,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="F1" s="36" t="s">
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="F1" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="K1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="K1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
       <c r="R1" s="1" t="s">
         <v>25</v>
       </c>
@@ -2459,10 +2468,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62F3CE8-EB31-4D8F-AAFD-E96DF7E64363}">
-  <dimension ref="B1:X74"/>
+  <dimension ref="B1:AE79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2480,27 +2489,42 @@
     <col min="17" max="16384" width="8.59765625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="36" t="s">
+    <row r="1" spans="2:31" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="F1" s="36" t="s">
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="F1" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="K1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-    </row>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="K1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="AA1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -2535,8 +2559,40 @@
       <c r="P2" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="S2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="36">
+        <f>SUM($H$3:H3)</f>
+        <v>600</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="W2" s="3">
+        <v>120</v>
+      </c>
+      <c r="X2" s="3">
+        <f>SUM($W$2:W2)</f>
+        <v>120</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z2" s="3" t="str">
+        <f>_xlfn.XLOOKUP(X2,$T$2:$T$6,$S$2:$S$6,,1)</f>
+        <v>P1</v>
+      </c>
+      <c r="AA2" s="36">
+        <f>IF($Y2=AA$1,IF(SUM($W$2:W2)&lt;=$H$3,W2,$H$3-SUM($W2:W$2)),"")</f>
+        <v>120</v>
+      </c>
+      <c r="AB2" s="3" t="str">
+        <f>IF(AND(AB$1&gt;=Y2,AB$1&lt;=Z2),IF(SUM($W$2:W2)&lt;=$H$3,W2,$H$3-SUM($W2:W$2)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>4</v>
       </c>
@@ -2565,8 +2621,40 @@
       <c r="N3" s="33"/>
       <c r="O3" s="14"/>
       <c r="P3" s="15"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="S3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="T3" s="36">
+        <f>SUM($H$3:H4)</f>
+        <v>650</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="W3" s="3">
+        <v>356</v>
+      </c>
+      <c r="X3" s="3">
+        <f>SUM($W$2:W3)</f>
+        <v>476</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z3" s="3" t="str">
+        <f t="shared" ref="Z3:Z13" si="0">_xlfn.XLOOKUP(X3,$T$2:$T$6,$S$2:$S$6,,1)</f>
+        <v>P1</v>
+      </c>
+      <c r="AA3" s="36">
+        <f>IF($Y3=AA$1,IF(SUM($W$2:W3)&lt;=$H$3,W3,$H$3-SUM($W$2:W2)),"")</f>
+        <v>356</v>
+      </c>
+      <c r="AB3" s="3" t="str">
+        <f>IF(AND(AB$1&gt;=Y3,AB$1&lt;=Z3),IF(SUM($W$2:W3)&lt;=$H$3,W3,$H$3-SUM($W$2:W3)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>5</v>
       </c>
@@ -2595,8 +2683,40 @@
       <c r="N4" s="33"/>
       <c r="O4" s="33"/>
       <c r="P4" s="34"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="S4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="T4" s="36">
+        <f>SUM($H$3:H5)</f>
+        <v>762</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="W4" s="3">
+        <v>312</v>
+      </c>
+      <c r="X4" s="3">
+        <f>SUM($W$2:W4)</f>
+        <v>788</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>P4</v>
+      </c>
+      <c r="AA4" s="36">
+        <f>IF($Y4=AA$1,IF(SUM($W$2:W4)&lt;=$H$3,W4,$H$3-SUM($W$2:W3)),"")</f>
+        <v>124</v>
+      </c>
+      <c r="AB4" s="3">
+        <f>IF(AND(AB$1&gt;=Y4,AB$1&lt;=Z4),IF(SUM($W$2:W4)&lt;=$H$3,W4,$H$3-SUM($W$2:W4)),"")</f>
+        <v>-188</v>
+      </c>
+    </row>
+    <row r="5" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
         <v>6</v>
       </c>
@@ -2631,8 +2751,40 @@
         <v>26</v>
       </c>
       <c r="P5" s="34"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="S5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="T5" s="36">
+        <f>SUM($H$3:H6)</f>
+        <v>1562</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="W5" s="3">
+        <v>437</v>
+      </c>
+      <c r="X5" s="3">
+        <f>SUM($W$2:W5)</f>
+        <v>1225</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>P4</v>
+      </c>
+      <c r="AA5" s="36" t="str">
+        <f>IF($Y5=AA$1,IF(SUM($W$2:W5)&lt;=$H$3,W5,$H$3-SUM($W$2:W4)),"")</f>
+        <v/>
+      </c>
+      <c r="AB5" s="3" t="str">
+        <f>IF(AND(AB$1&gt;=Y5,AB$1&lt;=Z5),IF(SUM($W$2:W5)&lt;=$H$3,W5,$H$3-SUM($W$2:W5)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>7</v>
       </c>
@@ -2661,8 +2813,40 @@
         <v>437</v>
       </c>
       <c r="P6" s="34"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="S6" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="T6" s="36">
+        <f>SUM($H$3:H7)</f>
+        <v>3362</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="W6" s="3">
+        <v>374</v>
+      </c>
+      <c r="X6" s="3">
+        <f>SUM($W$2:W6)</f>
+        <v>1599</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>P5</v>
+      </c>
+      <c r="AA6" s="36" t="str">
+        <f>IF($Y6=AA$1,IF(SUM($W$2:W6)&lt;=$H$3,W6,$H$3-SUM($W$2:W5)),"")</f>
+        <v/>
+      </c>
+      <c r="AB6" s="3" t="str">
+        <f>IF(AND(AB$1&gt;=Y6,AB$1&lt;=Z6),IF(SUM($W$2:W6)&lt;=$H$3,W6,$H$3-SUM($W$2:W6)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
@@ -2693,8 +2877,33 @@
       <c r="P7" s="34">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="V7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="W7" s="3">
+        <v>258</v>
+      </c>
+      <c r="X7" s="3">
+        <f>SUM($W$2:W7)</f>
+        <v>1857</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>P5</v>
+      </c>
+      <c r="AA7" s="36" t="str">
+        <f>IF($Y7=AA$1,IF(SUM($W$2:W7)&lt;=$H$3,W7,$H$3-SUM($W$2:W6)),"")</f>
+        <v/>
+      </c>
+      <c r="AB7" s="3" t="str">
+        <f>IF(AND(AB$1&gt;=Y7,AB$1&lt;=Z7),IF(SUM($W$2:W7)&lt;=$H$3,W7,$H$3-SUM($W$2:W7)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>9</v>
       </c>
@@ -2714,8 +2923,33 @@
       <c r="P8" s="34">
         <v>258</v>
       </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="V8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W8" s="3">
+        <v>369</v>
+      </c>
+      <c r="X8" s="3">
+        <f>SUM($W$2:W8)</f>
+        <v>2226</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>P5</v>
+      </c>
+      <c r="AA8" s="36" t="str">
+        <f>IF($Y8=AA$1,IF(SUM($W$2:W8)&lt;=$H$3,W8,$H$3-SUM($W$2:W7)),"")</f>
+        <v/>
+      </c>
+      <c r="AB8" s="3" t="str">
+        <f>IF(AND(AB$1&gt;=Y8,AB$1&lt;=Z8),IF(SUM($W$2:W8)&lt;=$H$3,W8,$H$3-SUM($W$2:W8)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>10</v>
       </c>
@@ -2735,8 +2969,33 @@
       <c r="P9" s="34">
         <v>369</v>
       </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="V9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="W9" s="3">
+        <v>418</v>
+      </c>
+      <c r="X9" s="3">
+        <f>SUM($W$2:W9)</f>
+        <v>2644</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>P5</v>
+      </c>
+      <c r="AA9" s="36" t="str">
+        <f>IF($Y9=AA$1,IF(SUM($W$2:W9)&lt;=$H$3,W9,$H$3-SUM($W$2:W8)),"")</f>
+        <v/>
+      </c>
+      <c r="AB9" s="3" t="str">
+        <f>IF(AND(AB$1&gt;=Y9,AB$1&lt;=Z9),IF(SUM($W$2:W9)&lt;=$H$3,W9,$H$3-SUM($W$2:W9)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>11</v>
       </c>
@@ -2756,8 +3015,33 @@
       <c r="P10" s="34">
         <v>418</v>
       </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="V10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="W10" s="3">
+        <v>308</v>
+      </c>
+      <c r="X10" s="3">
+        <f>SUM($W$2:W10)</f>
+        <v>2952</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>P5</v>
+      </c>
+      <c r="AA10" s="36" t="str">
+        <f>IF($Y10=AA$1,IF(SUM($W$2:W10)&lt;=$H$3,W10,$H$3-SUM($W$2:W9)),"")</f>
+        <v/>
+      </c>
+      <c r="AB10" s="3" t="str">
+        <f>IF(AND(AB$1&gt;=Y10,AB$1&lt;=Z10),IF(SUM($W$2:W10)&lt;=$H$3,W10,$H$3-SUM($W$2:W10)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>12</v>
       </c>
@@ -2777,8 +3061,33 @@
       <c r="P11" s="34">
         <v>308</v>
       </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="V11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="W11" s="3">
+        <v>410</v>
+      </c>
+      <c r="X11" s="3">
+        <f>SUM($W$2:W11)</f>
+        <v>3362</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>P5</v>
+      </c>
+      <c r="AA11" s="36" t="str">
+        <f>IF($Y11=AA$1,IF(SUM($W$2:W11)&lt;=$H$3,W11,$H$3-SUM($W$2:W10)),"")</f>
+        <v/>
+      </c>
+      <c r="AB11" s="3" t="str">
+        <f>IF(AND(AB$1&gt;=Y11,AB$1&lt;=Z11),IF(SUM($W$2:W11)&lt;=$H$3,W11,$H$3-SUM($W$2:W11)),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>13</v>
       </c>
@@ -2799,8 +3108,30 @@
       <c r="P12" s="34">
         <v>410</v>
       </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="V12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="W12" s="3">
+        <v>491</v>
+      </c>
+      <c r="X12" s="3">
+        <f>SUM($W$2:W12)</f>
+        <v>3853</v>
+      </c>
+      <c r="Z12" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA12" s="36" t="str">
+        <f>IF($Y12=AA$1,IF(SUM($W$2:W12)&lt;=$H$3,W12,$H$3-SUM($W$2:W11)),"")</f>
+        <v/>
+      </c>
+      <c r="AB12" s="3" t="e">
+        <f>IF(AND(AB$1&gt;=Y12,AB$1&lt;=Z12),IF(SUM($W$2:W12)&lt;=$H$3,W12,$H$3-SUM($W$2:W12)),"")</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>14</v>
       </c>
@@ -2829,8 +3160,30 @@
       <c r="P13" s="15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="V13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="W13" s="3">
+        <v>50</v>
+      </c>
+      <c r="X13" s="3">
+        <f>SUM($W$2:W13)</f>
+        <v>3903</v>
+      </c>
+      <c r="Z13" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA13" s="36" t="str">
+        <f>IF($Y13=AA$1,IF(SUM($W$2:W13)&lt;=$H$3,W13,$H$3-SUM($W$2:W12)),"")</f>
+        <v/>
+      </c>
+      <c r="AB13" s="3" t="e">
+        <f>IF(AND(AB$1&gt;=Y13,AB$1&lt;=Z13),IF(SUM($W$2:W13)&lt;=$H$3,W13,$H$3-SUM($W$2:W13)),"")</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>22</v>
       </c>
@@ -2860,14 +3213,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="G15" s="20"/>
       <c r="L15" s="27"/>
       <c r="O15" s="20"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:31" x14ac:dyDescent="0.25">
       <c r="G16" s="20"/>
       <c r="L16" s="27"/>
       <c r="O16" s="20"/>
@@ -2883,37 +3236,55 @@
       <c r="O18" s="20"/>
     </row>
     <row r="19" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
+      <c r="G19" s="20"/>
+      <c r="L19" s="27"/>
+      <c r="O19" s="20"/>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="G20" s="20"/>
+      <c r="L20" s="27"/>
+      <c r="O20" s="20"/>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="G21" s="20"/>
+      <c r="L21" s="27"/>
+      <c r="O21" s="20"/>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="G22" s="20"/>
+      <c r="L22" s="27"/>
+      <c r="O22" s="20"/>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="G23" s="20"/>
+      <c r="L23" s="27"/>
+      <c r="O23" s="20"/>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C24" s="10">
         <v>45325</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D24" s="29">
         <v>120</v>
       </c>
-      <c r="E19" s="3">
-        <f>SUMIF($G$3:$G$7,"&lt;="&amp;C19,$H$3:$H$7)</f>
+      <c r="E24" s="3">
+        <f>SUMIF($G$3:$G$7,"&lt;="&amp;C24,$H$3:$H$7)</f>
         <v>1562</v>
       </c>
-      <c r="F19" s="38">
-        <f>SUM($D$19:D19)</f>
+      <c r="F24" s="36">
+        <f>SUM($D$24:D24)</f>
         <v>120</v>
       </c>
-      <c r="G19" s="3" t="e">
-        <f>_xlfn.XLOOKUP(F19,$J$19:$J$23,$I$19:$I$23,,-1)</f>
+      <c r="G24" s="3" t="e">
+        <f>_xlfn.XLOOKUP(F24,$T$2:$T$6,$S$2:$S$6,,-1)</f>
         <v>#N/A</v>
       </c>
-      <c r="I19" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="J19" s="38">
-        <f>SUM($H$3:H3)</f>
-        <v>600</v>
-      </c>
-      <c r="L19" s="20"/>
-      <c r="N19" s="3" cm="1">
-        <f t="array" ref="N19:R30">_xlfn.LET(
+      <c r="L24" s="20"/>
+      <c r="N24" s="3" cm="1">
+        <f t="array" ref="N24:R35">_xlfn.LET(
 _xlpm.s,_xlfn.SEQUENCE(5),
 _xlpm.i,_xlfn.CHOOSECOLS(_xlfn.REDUCE(D3:D14,
                     H3:H7,
@@ -2922,20 +3293,20 @@
 _xlfn.HSTACK(_xlpm.a,_xlfn.IFS(_xlpm.e&gt;_xlpm.v,_xlpm.v,_xlpm.e&gt;0,_xlpm.e,1,),_xlfn.IFS(_xlpm.e&gt;_xlpm.v,0,_xlpm.e&lt;0,_xlpm.v,1,_xlpm.v-_xlpm.e))))),_xlpm.s*2),IF(MMULT(_xlpm.i,_xlpm.s^0),_xlpm.i,"NP"))</f>
         <v>120</v>
       </c>
-      <c r="O19" s="20">
-        <v>0</v>
-      </c>
-      <c r="P19" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="3">
-        <v>0</v>
-      </c>
-      <c r="R19" s="3">
-        <v>0</v>
-      </c>
-      <c r="T19" s="3" cm="1">
-        <f t="array" ref="T19:X30">_xlfn.LET(
+      <c r="O24" s="20">
+        <v>0</v>
+      </c>
+      <c r="P24" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>0</v>
+      </c>
+      <c r="R24" s="3">
+        <v>0</v>
+      </c>
+      <c r="T24" s="3" cm="1">
+        <f t="array" ref="T24:X35">_xlfn.LET(
 _xlpm.s,_xlfn.SEQUENCE(5),
 _xlpm.i,_xlfn.CHOOSECOLS(_xlfn.REDUCE(D3:D14,
                     H3:H7,
@@ -2945,304 +3316,6 @@
 _xlpm.i)</f>
         <v>120</v>
       </c>
-      <c r="U19" s="3">
-        <v>0</v>
-      </c>
-      <c r="V19" s="3">
-        <v>0</v>
-      </c>
-      <c r="W19" s="3">
-        <v>0</v>
-      </c>
-      <c r="X19" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B20" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="16">
-        <v>45338</v>
-      </c>
-      <c r="D20" s="30">
-        <v>356</v>
-      </c>
-      <c r="E20" s="3">
-        <f t="shared" ref="E20:E30" si="0">SUMIF($G$3:$G$7,"&lt;="&amp;C20,$H$3:$H$7)</f>
-        <v>3362</v>
-      </c>
-      <c r="F20" s="38">
-        <f>SUM($D$19:D20)</f>
-        <v>476</v>
-      </c>
-      <c r="G20" s="3" t="e">
-        <f t="shared" ref="G20:G30" si="1">_xlfn.XLOOKUP(F20,$J$19:$J$23,$I$19:$I$23,,-1)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J20" s="38">
-        <f>SUM($H$3:H4)</f>
-        <v>650</v>
-      </c>
-      <c r="L20" s="20"/>
-      <c r="N20" s="3">
-        <v>356</v>
-      </c>
-      <c r="O20" s="20">
-        <v>0</v>
-      </c>
-      <c r="P20" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="3">
-        <v>0</v>
-      </c>
-      <c r="R20" s="3">
-        <v>0</v>
-      </c>
-      <c r="T20" s="3">
-        <v>356</v>
-      </c>
-      <c r="U20" s="3">
-        <v>0</v>
-      </c>
-      <c r="V20" s="3">
-        <v>0</v>
-      </c>
-      <c r="W20" s="3">
-        <v>0</v>
-      </c>
-      <c r="X20" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B21" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="16">
-        <v>45341</v>
-      </c>
-      <c r="D21" s="30">
-        <v>312</v>
-      </c>
-      <c r="E21" s="3">
-        <f t="shared" si="0"/>
-        <v>3362</v>
-      </c>
-      <c r="F21" s="38">
-        <f>SUM($D$19:D21)</f>
-        <v>788</v>
-      </c>
-      <c r="G21" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>P3</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="38">
-        <f>SUM($H$3:H5)</f>
-        <v>762</v>
-      </c>
-      <c r="L21" s="20"/>
-      <c r="N21" s="3">
-        <v>124</v>
-      </c>
-      <c r="O21" s="20">
-        <v>50</v>
-      </c>
-      <c r="P21" s="3">
-        <v>112</v>
-      </c>
-      <c r="Q21" s="3">
-        <v>26</v>
-      </c>
-      <c r="R21" s="3">
-        <v>0</v>
-      </c>
-      <c r="T21" s="3">
-        <v>124</v>
-      </c>
-      <c r="U21" s="3">
-        <v>50</v>
-      </c>
-      <c r="V21" s="3">
-        <v>112</v>
-      </c>
-      <c r="W21" s="3">
-        <v>26</v>
-      </c>
-      <c r="X21" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="16">
-        <v>45355</v>
-      </c>
-      <c r="D22" s="30">
-        <v>437</v>
-      </c>
-      <c r="E22" s="3">
-        <f t="shared" si="0"/>
-        <v>3362</v>
-      </c>
-      <c r="F22" s="38">
-        <f>SUM($D$19:D22)</f>
-        <v>1225</v>
-      </c>
-      <c r="G22" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>P3</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J22" s="38">
-        <f>SUM($H$3:H6)</f>
-        <v>1562</v>
-      </c>
-      <c r="L22" s="20"/>
-      <c r="N22" s="3">
-        <v>0</v>
-      </c>
-      <c r="O22" s="20">
-        <v>0</v>
-      </c>
-      <c r="P22" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="3">
-        <v>437</v>
-      </c>
-      <c r="R22" s="3">
-        <v>0</v>
-      </c>
-      <c r="T22" s="3">
-        <v>0</v>
-      </c>
-      <c r="U22" s="3">
-        <v>0</v>
-      </c>
-      <c r="V22" s="3">
-        <v>0</v>
-      </c>
-      <c r="W22" s="3">
-        <v>437</v>
-      </c>
-      <c r="X22" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B23" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="16">
-        <v>45364</v>
-      </c>
-      <c r="D23" s="30">
-        <v>374</v>
-      </c>
-      <c r="E23" s="3">
-        <f t="shared" si="0"/>
-        <v>3362</v>
-      </c>
-      <c r="F23" s="38">
-        <f>SUM($D$19:D23)</f>
-        <v>1599</v>
-      </c>
-      <c r="G23" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>P4</v>
-      </c>
-      <c r="I23" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="J23" s="38">
-        <f>SUM($H$3:H7)</f>
-        <v>3362</v>
-      </c>
-      <c r="L23" s="20"/>
-      <c r="N23" s="3">
-        <v>0</v>
-      </c>
-      <c r="O23" s="20">
-        <v>0</v>
-      </c>
-      <c r="P23" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="3">
-        <v>337</v>
-      </c>
-      <c r="R23" s="3">
-        <v>37</v>
-      </c>
-      <c r="T23" s="3">
-        <v>0</v>
-      </c>
-      <c r="U23" s="3">
-        <v>0</v>
-      </c>
-      <c r="V23" s="3">
-        <v>0</v>
-      </c>
-      <c r="W23" s="3">
-        <v>337</v>
-      </c>
-      <c r="X23" s="3">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="16">
-        <v>45365</v>
-      </c>
-      <c r="D24" s="30">
-        <v>258</v>
-      </c>
-      <c r="E24" s="3">
-        <f t="shared" si="0"/>
-        <v>3362</v>
-      </c>
-      <c r="F24" s="38">
-        <f>SUM($D$19:D24)</f>
-        <v>1857</v>
-      </c>
-      <c r="G24" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>P4</v>
-      </c>
-      <c r="L24" s="20"/>
-      <c r="N24" s="3">
-        <v>0</v>
-      </c>
-      <c r="O24" s="20">
-        <v>0</v>
-      </c>
-      <c r="P24" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="3">
-        <v>0</v>
-      </c>
-      <c r="R24" s="3">
-        <v>258</v>
-      </c>
-      <c r="T24" s="3">
-        <v>0</v>
-      </c>
       <c r="U24" s="3">
         <v>0</v>
       </c>
@@ -3253,34 +3326,34 @@
         <v>0</v>
       </c>
       <c r="X24" s="3">
-        <v>258</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C25" s="16">
-        <v>45370</v>
+        <v>45338</v>
       </c>
       <c r="D25" s="30">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="E25" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E25:E35" si="1">SUMIF($G$3:$G$7,"&lt;="&amp;C25,$H$3:$H$7)</f>
         <v>3362</v>
       </c>
-      <c r="F25" s="38">
-        <f>SUM($D$19:D25)</f>
-        <v>2226</v>
-      </c>
-      <c r="G25" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>P4</v>
+      <c r="F25" s="36">
+        <f>SUM($D$24:D25)</f>
+        <v>476</v>
+      </c>
+      <c r="G25" s="3" t="e">
+        <f>_xlfn.XLOOKUP(F25,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <v>#N/A</v>
       </c>
       <c r="L25" s="20"/>
       <c r="N25" s="3">
-        <v>0</v>
+        <v>356</v>
       </c>
       <c r="O25" s="20">
         <v>0</v>
@@ -3292,10 +3365,10 @@
         <v>0</v>
       </c>
       <c r="R25" s="3">
-        <v>369</v>
+        <v>0</v>
       </c>
       <c r="T25" s="3">
-        <v>0</v>
+        <v>356</v>
       </c>
       <c r="U25" s="3">
         <v>0</v>
@@ -3307,84 +3380,84 @@
         <v>0</v>
       </c>
       <c r="X25" s="3">
-        <v>369</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C26" s="16">
-        <v>45376</v>
+        <v>45341</v>
       </c>
       <c r="D26" s="30">
-        <v>418</v>
+        <v>312</v>
       </c>
       <c r="E26" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3362</v>
       </c>
-      <c r="F26" s="38">
-        <f>SUM($D$19:D26)</f>
-        <v>2644</v>
+      <c r="F26" s="36">
+        <f>SUM($D$24:D26)</f>
+        <v>788</v>
       </c>
       <c r="G26" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>P4</v>
+        <f>_xlfn.XLOOKUP(F26,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <v>P3</v>
       </c>
       <c r="L26" s="20"/>
       <c r="N26" s="3">
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="O26" s="20">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P26" s="3">
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="Q26" s="3">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="R26" s="3">
-        <v>418</v>
+        <v>0</v>
       </c>
       <c r="T26" s="3">
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="U26" s="3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="V26" s="3">
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="W26" s="3">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="X26" s="3">
-        <v>418</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C27" s="16">
-        <v>45384</v>
+        <v>45355</v>
       </c>
       <c r="D27" s="30">
-        <v>308</v>
+        <v>437</v>
       </c>
       <c r="E27" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3362</v>
       </c>
-      <c r="F27" s="38">
-        <f>SUM($D$19:D27)</f>
-        <v>2952</v>
+      <c r="F27" s="36">
+        <f>SUM($D$24:D27)</f>
+        <v>1225</v>
       </c>
       <c r="G27" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>P4</v>
+        <f>_xlfn.XLOOKUP(F27,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <v>P3</v>
       </c>
       <c r="L27" s="20"/>
       <c r="N27" s="3">
@@ -3397,10 +3470,10 @@
         <v>0</v>
       </c>
       <c r="Q27" s="3">
-        <v>0</v>
+        <v>437</v>
       </c>
       <c r="R27" s="3">
-        <v>308</v>
+        <v>0</v>
       </c>
       <c r="T27" s="3">
         <v>0</v>
@@ -3412,33 +3485,33 @@
         <v>0</v>
       </c>
       <c r="W27" s="3">
-        <v>0</v>
+        <v>437</v>
       </c>
       <c r="X27" s="3">
-        <v>308</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C28" s="16">
-        <v>45397</v>
+        <v>45364</v>
       </c>
       <c r="D28" s="30">
-        <v>410</v>
+        <v>374</v>
       </c>
       <c r="E28" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3362</v>
       </c>
-      <c r="F28" s="38">
-        <f>SUM($D$19:D28)</f>
-        <v>3362</v>
+      <c r="F28" s="36">
+        <f>SUM($D$24:D28)</f>
+        <v>1599</v>
       </c>
       <c r="G28" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>P5</v>
+        <f>_xlfn.XLOOKUP(F28,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <v>P4</v>
       </c>
       <c r="L28" s="20"/>
       <c r="N28" s="3">
@@ -3451,10 +3524,10 @@
         <v>0</v>
       </c>
       <c r="Q28" s="3">
-        <v>0</v>
+        <v>337</v>
       </c>
       <c r="R28" s="3">
-        <v>410</v>
+        <v>37</v>
       </c>
       <c r="T28" s="3">
         <v>0</v>
@@ -3466,48 +3539,49 @@
         <v>0</v>
       </c>
       <c r="W28" s="3">
-        <v>0</v>
+        <v>337</v>
       </c>
       <c r="X28" s="3">
-        <v>410</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C29" s="16">
-        <v>45406</v>
+        <v>45365</v>
       </c>
       <c r="D29" s="30">
-        <v>491</v>
+        <v>258</v>
       </c>
       <c r="E29" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3362</v>
       </c>
-      <c r="F29" s="38">
-        <f>SUM($D$19:D29)</f>
-        <v>3853</v>
+      <c r="F29" s="36">
+        <f>SUM($D$24:D29)</f>
+        <v>1857</v>
       </c>
       <c r="G29" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>P5</v>
-      </c>
-      <c r="N29" s="3" t="str">
-        <v>NP</v>
-      </c>
-      <c r="O29" s="20" t="str">
-        <v>NP</v>
-      </c>
-      <c r="P29" s="3" t="str">
-        <v>NP</v>
-      </c>
-      <c r="Q29" s="3" t="str">
-        <v>NP</v>
-      </c>
-      <c r="R29" s="3" t="str">
-        <v>NP</v>
+        <f>_xlfn.XLOOKUP(F29,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <v>P4</v>
+      </c>
+      <c r="L29" s="20"/>
+      <c r="N29" s="3">
+        <v>0</v>
+      </c>
+      <c r="O29" s="20">
+        <v>0</v>
+      </c>
+      <c r="P29" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>0</v>
+      </c>
+      <c r="R29" s="3">
+        <v>258</v>
       </c>
       <c r="T29" s="3">
         <v>0</v>
@@ -3522,114 +3596,368 @@
         <v>0</v>
       </c>
       <c r="X29" s="3">
-        <v>0</v>
+        <v>258</v>
       </c>
     </row>
     <row r="30" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="16">
+        <v>45370</v>
+      </c>
+      <c r="D30" s="30">
+        <v>369</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="1"/>
+        <v>3362</v>
+      </c>
+      <c r="F30" s="36">
+        <f>SUM($D$24:D30)</f>
+        <v>2226</v>
+      </c>
+      <c r="G30" s="3" t="str">
+        <f>_xlfn.XLOOKUP(F30,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <v>P4</v>
+      </c>
+      <c r="L30" s="20"/>
+      <c r="N30" s="3">
+        <v>0</v>
+      </c>
+      <c r="O30" s="20">
+        <v>0</v>
+      </c>
+      <c r="P30" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>0</v>
+      </c>
+      <c r="R30" s="3">
+        <v>369</v>
+      </c>
+      <c r="T30" s="3">
+        <v>0</v>
+      </c>
+      <c r="U30" s="3">
+        <v>0</v>
+      </c>
+      <c r="V30" s="3">
+        <v>0</v>
+      </c>
+      <c r="W30" s="3">
+        <v>0</v>
+      </c>
+      <c r="X30" s="3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B31" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="16">
+        <v>45376</v>
+      </c>
+      <c r="D31" s="30">
+        <v>418</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="1"/>
+        <v>3362</v>
+      </c>
+      <c r="F31" s="36">
+        <f>SUM($D$24:D31)</f>
+        <v>2644</v>
+      </c>
+      <c r="G31" s="3" t="str">
+        <f>_xlfn.XLOOKUP(F31,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <v>P4</v>
+      </c>
+      <c r="L31" s="20"/>
+      <c r="N31" s="3">
+        <v>0</v>
+      </c>
+      <c r="O31" s="20">
+        <v>0</v>
+      </c>
+      <c r="P31" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>0</v>
+      </c>
+      <c r="R31" s="3">
+        <v>418</v>
+      </c>
+      <c r="T31" s="3">
+        <v>0</v>
+      </c>
+      <c r="U31" s="3">
+        <v>0</v>
+      </c>
+      <c r="V31" s="3">
+        <v>0</v>
+      </c>
+      <c r="W31" s="3">
+        <v>0</v>
+      </c>
+      <c r="X31" s="3">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="16">
+        <v>45384</v>
+      </c>
+      <c r="D32" s="30">
+        <v>308</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="1"/>
+        <v>3362</v>
+      </c>
+      <c r="F32" s="36">
+        <f>SUM($D$24:D32)</f>
+        <v>2952</v>
+      </c>
+      <c r="G32" s="3" t="str">
+        <f>_xlfn.XLOOKUP(F32,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <v>P4</v>
+      </c>
+      <c r="L32" s="20"/>
+      <c r="N32" s="3">
+        <v>0</v>
+      </c>
+      <c r="O32" s="20">
+        <v>0</v>
+      </c>
+      <c r="P32" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>0</v>
+      </c>
+      <c r="R32" s="3">
+        <v>308</v>
+      </c>
+      <c r="T32" s="3">
+        <v>0</v>
+      </c>
+      <c r="U32" s="3">
+        <v>0</v>
+      </c>
+      <c r="V32" s="3">
+        <v>0</v>
+      </c>
+      <c r="W32" s="3">
+        <v>0</v>
+      </c>
+      <c r="X32" s="3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="33" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B33" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="16">
+        <v>45397</v>
+      </c>
+      <c r="D33" s="30">
+        <v>410</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="1"/>
+        <v>3362</v>
+      </c>
+      <c r="F33" s="36">
+        <f>SUM($D$24:D33)</f>
+        <v>3362</v>
+      </c>
+      <c r="G33" s="3" t="str">
+        <f>_xlfn.XLOOKUP(F33,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <v>P5</v>
+      </c>
+      <c r="L33" s="20"/>
+      <c r="N33" s="3">
+        <v>0</v>
+      </c>
+      <c r="O33" s="20">
+        <v>0</v>
+      </c>
+      <c r="P33" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>0</v>
+      </c>
+      <c r="R33" s="3">
+        <v>410</v>
+      </c>
+      <c r="T33" s="3">
+        <v>0</v>
+      </c>
+      <c r="U33" s="3">
+        <v>0</v>
+      </c>
+      <c r="V33" s="3">
+        <v>0</v>
+      </c>
+      <c r="W33" s="3">
+        <v>0</v>
+      </c>
+      <c r="X33" s="3">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="34" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B34" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="16">
+        <v>45406</v>
+      </c>
+      <c r="D34" s="30">
+        <v>491</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="1"/>
+        <v>3362</v>
+      </c>
+      <c r="F34" s="36">
+        <f>SUM($D$24:D34)</f>
+        <v>3853</v>
+      </c>
+      <c r="G34" s="3" t="str">
+        <f>_xlfn.XLOOKUP(F34,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <v>P5</v>
+      </c>
+      <c r="N34" s="3" t="str">
+        <v>NP</v>
+      </c>
+      <c r="O34" s="20" t="str">
+        <v>NP</v>
+      </c>
+      <c r="P34" s="3" t="str">
+        <v>NP</v>
+      </c>
+      <c r="Q34" s="3" t="str">
+        <v>NP</v>
+      </c>
+      <c r="R34" s="3" t="str">
+        <v>NP</v>
+      </c>
+      <c r="T34" s="3">
+        <v>0</v>
+      </c>
+      <c r="U34" s="3">
+        <v>0</v>
+      </c>
+      <c r="V34" s="3">
+        <v>0</v>
+      </c>
+      <c r="W34" s="3">
+        <v>0</v>
+      </c>
+      <c r="X34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B35" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C30" s="16">
+      <c r="C35" s="16">
         <v>45409</v>
       </c>
-      <c r="D30" s="30">
+      <c r="D35" s="30">
         <v>50</v>
       </c>
-      <c r="E30" s="3">
-        <f t="shared" si="0"/>
+      <c r="E35" s="3">
+        <f t="shared" si="1"/>
         <v>3362</v>
       </c>
-      <c r="F30" s="38">
-        <f>SUM($D$19:D30)</f>
+      <c r="F35" s="36">
+        <f>SUM($D$24:D35)</f>
         <v>3903</v>
       </c>
-      <c r="G30" s="3" t="str">
-        <f t="shared" si="1"/>
+      <c r="G35" s="3" t="str">
+        <f>_xlfn.XLOOKUP(F35,$T$2:$T$6,$S$2:$S$6,,-1)</f>
         <v>P5</v>
       </c>
-      <c r="N30" s="3" t="str">
+      <c r="N35" s="3" t="str">
         <v>NP</v>
       </c>
-      <c r="O30" s="20" t="str">
+      <c r="O35" s="20" t="str">
         <v>NP</v>
       </c>
-      <c r="P30" s="3" t="str">
+      <c r="P35" s="3" t="str">
         <v>NP</v>
       </c>
-      <c r="Q30" s="3" t="str">
+      <c r="Q35" s="3" t="str">
         <v>NP</v>
       </c>
-      <c r="R30" s="3" t="str">
+      <c r="R35" s="3" t="str">
         <v>NP</v>
       </c>
-      <c r="T30" s="3">
-        <v>0</v>
-      </c>
-      <c r="U30" s="3">
-        <v>0</v>
-      </c>
-      <c r="V30" s="3">
-        <v>0</v>
-      </c>
-      <c r="W30" s="3">
-        <v>0</v>
-      </c>
-      <c r="X30" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="O31" s="20"/>
-    </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="O32" s="20"/>
-    </row>
-    <row r="33" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O33" s="20"/>
-    </row>
-    <row r="34" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O34" s="20"/>
-    </row>
-    <row r="35" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O35" s="20"/>
-    </row>
-    <row r="36" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="T35" s="3">
+        <v>0</v>
+      </c>
+      <c r="U35" s="3">
+        <v>0</v>
+      </c>
+      <c r="V35" s="3">
+        <v>0</v>
+      </c>
+      <c r="W35" s="3">
+        <v>0</v>
+      </c>
+      <c r="X35" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:24" x14ac:dyDescent="0.25">
       <c r="O36" s="20"/>
     </row>
-    <row r="37" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:24" x14ac:dyDescent="0.25">
       <c r="O37" s="20"/>
     </row>
-    <row r="38" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:24" x14ac:dyDescent="0.25">
       <c r="O38" s="20"/>
     </row>
-    <row r="39" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:24" x14ac:dyDescent="0.25">
       <c r="O39" s="20"/>
     </row>
-    <row r="40" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:24" x14ac:dyDescent="0.25">
       <c r="O40" s="20"/>
     </row>
-    <row r="41" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:24" x14ac:dyDescent="0.25">
       <c r="O41" s="20"/>
     </row>
-    <row r="42" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:24" x14ac:dyDescent="0.25">
       <c r="O42" s="20"/>
     </row>
-    <row r="43" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:24" x14ac:dyDescent="0.25">
       <c r="O43" s="20"/>
     </row>
-    <row r="44" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:24" x14ac:dyDescent="0.25">
       <c r="O44" s="20"/>
     </row>
-    <row r="45" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:24" x14ac:dyDescent="0.25">
       <c r="O45" s="20"/>
     </row>
-    <row r="46" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:24" x14ac:dyDescent="0.25">
       <c r="O46" s="20"/>
     </row>
-    <row r="47" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:24" x14ac:dyDescent="0.25">
       <c r="O47" s="20"/>
     </row>
-    <row r="48" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:24" x14ac:dyDescent="0.25">
       <c r="O48" s="20"/>
     </row>
     <row r="49" spans="15:15" x14ac:dyDescent="0.25">
@@ -3709,6 +4037,21 @@
     </row>
     <row r="74" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O74" s="20"/>
+    </row>
+    <row r="75" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O75" s="20"/>
+    </row>
+    <row r="76" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O76" s="20"/>
+    </row>
+    <row r="77" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O77" s="20"/>
+    </row>
+    <row r="78" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O78" s="20"/>
+    </row>
+    <row r="79" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O79" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3716,6 +4059,7 @@
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="K1:P1"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3726,7 +4070,7 @@
   <dimension ref="B1:R74"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3746,25 +4090,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="F1" s="36" t="s">
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="F1" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="K1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="R1" s="39" t="s">
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="K1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="R1" s="37" t="s">
         <v>25</v>
       </c>
     </row>
@@ -4836,8 +5180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D4DF196-8AFA-4D1D-A7A2-D917C2856F88}">
   <dimension ref="B1:Q74"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M63" sqref="M63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4856,24 +5200,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="F1" s="36" t="s">
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="F1" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="K1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="K1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -5446,6 +5790,1421 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D8F953-0749-4436-8A06-19D4F87E6D90}">
+  <dimension ref="B1:W73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q34" sqref="Q34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" style="3" customWidth="1"/>
+    <col min="2" max="2" width="4.09765625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="12.19921875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="6.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.59765625" style="3"/>
+    <col min="6" max="6" width="4.19921875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.8984375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="13.09765625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.59765625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="10.296875" style="3" customWidth="1"/>
+    <col min="13" max="16" width="6" style="3" customWidth="1"/>
+    <col min="17" max="21" width="8.59765625" style="3"/>
+    <col min="22" max="22" width="9" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.59765625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:22" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="F1" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="K1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="R1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="7"/>
+      <c r="L2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="10">
+        <v>45325</v>
+      </c>
+      <c r="D3" s="29">
+        <v>120</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="12">
+        <v>45278</v>
+      </c>
+      <c r="H3" s="31">
+        <v>600</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="33">
+        <v>120</v>
+      </c>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="15"/>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="16">
+        <v>45338</v>
+      </c>
+      <c r="D4" s="30">
+        <v>356</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="12">
+        <v>45286</v>
+      </c>
+      <c r="H4" s="31">
+        <v>50</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="33">
+        <v>356</v>
+      </c>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="34"/>
+      <c r="R4" s="40">
+        <v>1</v>
+      </c>
+      <c r="S4" s="40">
+        <v>2</v>
+      </c>
+      <c r="T4" s="40">
+        <v>3</v>
+      </c>
+      <c r="V4" s="3" cm="1">
+        <f t="array" ref="V4:V6">_xlfn.BYROW(R4:T6,_xlfn.LAMBDA(_xlpm.r,SUM(_xlpm.r)))</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="16">
+        <v>45341</v>
+      </c>
+      <c r="D5" s="30">
+        <v>312</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="12">
+        <v>45312</v>
+      </c>
+      <c r="H5" s="31">
+        <v>112</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="33">
+        <v>124</v>
+      </c>
+      <c r="M5" s="33">
+        <v>50</v>
+      </c>
+      <c r="N5" s="33">
+        <v>112</v>
+      </c>
+      <c r="O5" s="33">
+        <v>26</v>
+      </c>
+      <c r="P5" s="34"/>
+      <c r="R5" s="41">
+        <v>4</v>
+      </c>
+      <c r="S5" s="41">
+        <v>5</v>
+      </c>
+      <c r="T5" s="41">
+        <v>6</v>
+      </c>
+      <c r="V5" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="16">
+        <v>45355</v>
+      </c>
+      <c r="D6" s="30">
+        <v>437</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="12">
+        <v>45315</v>
+      </c>
+      <c r="H6" s="31">
+        <v>800</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33">
+        <v>437</v>
+      </c>
+      <c r="P6" s="34"/>
+      <c r="R6" s="40">
+        <v>7</v>
+      </c>
+      <c r="S6" s="40">
+        <v>8</v>
+      </c>
+      <c r="T6" s="40">
+        <v>9</v>
+      </c>
+      <c r="V6" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="16">
+        <v>45364</v>
+      </c>
+      <c r="D7" s="30">
+        <v>374</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="19">
+        <v>45327</v>
+      </c>
+      <c r="H7" s="32">
+        <v>1800</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33">
+        <v>337</v>
+      </c>
+      <c r="P7" s="34">
+        <v>37</v>
+      </c>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="16">
+        <v>45365</v>
+      </c>
+      <c r="D8" s="30">
+        <v>258</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="34">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="16">
+        <v>45370</v>
+      </c>
+      <c r="D9" s="30">
+        <v>369</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="17"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="34">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="16">
+        <v>45376</v>
+      </c>
+      <c r="D10" s="30">
+        <v>418</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="17"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="34">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="16">
+        <v>45384</v>
+      </c>
+      <c r="D11" s="30">
+        <v>308</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="17"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="34">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="16">
+        <v>45397</v>
+      </c>
+      <c r="D12" s="30">
+        <v>410</v>
+      </c>
+      <c r="G12" s="20"/>
+      <c r="K12" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="17"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="34">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="16">
+        <v>45406</v>
+      </c>
+      <c r="D13" s="30">
+        <v>491</v>
+      </c>
+      <c r="G13" s="20"/>
+      <c r="K13" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="P13" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="16">
+        <v>45409</v>
+      </c>
+      <c r="D14" s="30">
+        <v>50</v>
+      </c>
+      <c r="G14" s="20"/>
+      <c r="K14" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="O14" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="P14" s="26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="G15" s="20"/>
+      <c r="L15" s="27"/>
+      <c r="O15" s="20"/>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="G16" s="20"/>
+      <c r="L16" s="27"/>
+      <c r="O16" s="20"/>
+      <c r="R16" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="G17" s="20"/>
+      <c r="L17" s="27"/>
+      <c r="O17" s="20"/>
+    </row>
+    <row r="18" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="G18" s="20"/>
+      <c r="L18" s="27"/>
+      <c r="O18" s="20"/>
+    </row>
+    <row r="19" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="G19" s="3" t="str" cm="1">
+        <f t="array" ref="G19:L31">_xlfn.LET(
+    _xlpm.d, _xlfn.DROP(
+        _xlfn.REDUCE(
+            B3:B14,
+            H3:H7,
+            _xlfn.LAMBDA(_xlpm.b,_xlpm.w,
+                _xlfn.HSTACK(
+                    _xlpm.b,
+                    _xlfn.DROP(
+                        _xlfn.REDUCE(
+                            _xlpm.w,
+                            D3:D14 - _xlfn.BYROW(D3:D14, _xlfn.LAMBDA(_xlpm.r,SUM(_xlpm.r))),
+                            _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.VSTACK(_xlpm.a, MIN(_xlfn.SINGLE(_xlpm.a) * 2 - SUM(_xlpm.a), _xlpm.v)))
+                        ),
+                        1
+                    )
+                )
+            )
+        ),
+        ,
+        0
+    ),
+    _xlfn.VSTACK(_xlfn.TOROW(F2:F7), IF(_xlfn.BYROW(_xlpm.d, SUM) + (_xlpm.d &gt; ""), _xlpm.d, "NP")))</f>
+        <v>ID</v>
+      </c>
+      <c r="H19" s="3" t="str">
+        <v>P1</v>
+      </c>
+      <c r="I19" s="3" t="str">
+        <v>P2</v>
+      </c>
+      <c r="J19" s="36" t="str">
+        <v>P3</v>
+      </c>
+      <c r="K19" s="3" t="str">
+        <v>P4</v>
+      </c>
+      <c r="L19" s="20" t="str">
+        <v>P5</v>
+      </c>
+      <c r="O19" s="20" t="e" cm="1">
+        <f t="array" ref="O19">_xlfn.LET(_xlpm.d,_xlfn.DROP(_xlfn.REDUCE(B3:B14,H3:H7,_xlfn.LAMBDA(_xlpm.b,_xlpm.w,_xlfn.HSTACK(_xlpm.b,_xlfn.DROP(
+_xlfn.REDUCE(_xlpm.w,D3:D14-_xlfn.BYROW(_xlpm.b,SUM),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,MIN(_xlfn.SINGLE(_xlpm.a)*2-SUM(_xlpm.a),_xlpm.v)))),1)))),,0),
+_xlfn.VSTACK(_xlfn.TOROW(F2:F7),IF(_xlfn.BYROW(_xlpm.d,SUM)+(_xlpm.d&gt;""),_xlpm.d,"NP")))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="R19" s="3" t="str" cm="1">
+        <f t="array" ref="R19:W30">_xlfn.REDUCE(    B3:B14,
+            H3:H7,
+            _xlfn.LAMBDA(_xlpm.b,_xlpm.w,
+                _xlfn.HSTACK(
+                    _xlpm.b,
+                    _xlfn.DROP(
+                        _xlfn.REDUCE(
+                            _xlpm.w,
+                            D3:D14 - _xlfn.BYROW(_xlpm.b, _xlfn.LAMBDA(_xlpm.r,SUM(_xlpm.r))),
+                            _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.VSTACK(_xlpm.a, MIN(_xlfn.SINGLE(_xlpm.a) * 2 - SUM(_xlpm.a), _xlpm.v)))
+                        ),
+                        1
+                    )
+                )
+            )
+)</f>
+        <v>C1</v>
+      </c>
+      <c r="S19" s="3">
+        <v>120</v>
+      </c>
+      <c r="T19" s="3">
+        <v>0</v>
+      </c>
+      <c r="U19" s="3">
+        <v>0</v>
+      </c>
+      <c r="V19" s="3">
+        <v>0</v>
+      </c>
+      <c r="W19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="G20" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="H20" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="I20" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="J20" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="K20" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="L20" s="20" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="O20" s="20"/>
+      <c r="R20" s="3" t="str">
+        <v>C2</v>
+      </c>
+      <c r="S20" s="3">
+        <v>356</v>
+      </c>
+      <c r="T20" s="3">
+        <v>0</v>
+      </c>
+      <c r="U20" s="3">
+        <v>0</v>
+      </c>
+      <c r="V20" s="3">
+        <v>0</v>
+      </c>
+      <c r="W20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="G21" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="H21" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="I21" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="J21" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="K21" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="L21" s="20" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="O21" s="20"/>
+      <c r="R21" s="3" t="str">
+        <v>C3</v>
+      </c>
+      <c r="S21" s="3">
+        <v>124</v>
+      </c>
+      <c r="T21" s="3">
+        <v>50</v>
+      </c>
+      <c r="U21" s="3">
+        <v>112</v>
+      </c>
+      <c r="V21" s="3">
+        <v>26</v>
+      </c>
+      <c r="W21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="G22" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="H22" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="I22" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="J22" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="K22" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="L22" s="20" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="O22" s="20"/>
+      <c r="R22" s="3" t="str">
+        <v>C4</v>
+      </c>
+      <c r="S22" s="3">
+        <v>0</v>
+      </c>
+      <c r="T22" s="3">
+        <v>0</v>
+      </c>
+      <c r="U22" s="3">
+        <v>0</v>
+      </c>
+      <c r="V22" s="3">
+        <v>437</v>
+      </c>
+      <c r="W22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="G23" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="H23" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="I23" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="J23" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="K23" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="L23" s="20" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="O23" s="20"/>
+      <c r="R23" s="3" t="str">
+        <v>C5</v>
+      </c>
+      <c r="S23" s="3">
+        <v>0</v>
+      </c>
+      <c r="T23" s="3">
+        <v>0</v>
+      </c>
+      <c r="U23" s="3">
+        <v>0</v>
+      </c>
+      <c r="V23" s="3">
+        <v>337</v>
+      </c>
+      <c r="W23" s="3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="G24" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="H24" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="I24" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="J24" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="K24" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="L24" s="20" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="O24" s="20"/>
+      <c r="R24" s="3" t="str">
+        <v>C6</v>
+      </c>
+      <c r="S24" s="3">
+        <v>0</v>
+      </c>
+      <c r="T24" s="3">
+        <v>0</v>
+      </c>
+      <c r="U24" s="3">
+        <v>0</v>
+      </c>
+      <c r="V24" s="3">
+        <v>0</v>
+      </c>
+      <c r="W24" s="3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="25" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="G25" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="H25" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="I25" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="J25" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="K25" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="L25" s="20" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="O25" s="20"/>
+      <c r="R25" s="3" t="str">
+        <v>C7</v>
+      </c>
+      <c r="S25" s="3">
+        <v>0</v>
+      </c>
+      <c r="T25" s="3">
+        <v>0</v>
+      </c>
+      <c r="U25" s="3">
+        <v>0</v>
+      </c>
+      <c r="V25" s="3">
+        <v>0</v>
+      </c>
+      <c r="W25" s="3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="26" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="G26" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="H26" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="I26" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="J26" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="K26" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="L26" s="20" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="O26" s="20"/>
+      <c r="R26" s="3" t="str">
+        <v>C8</v>
+      </c>
+      <c r="S26" s="3">
+        <v>0</v>
+      </c>
+      <c r="T26" s="3">
+        <v>0</v>
+      </c>
+      <c r="U26" s="3">
+        <v>0</v>
+      </c>
+      <c r="V26" s="3">
+        <v>0</v>
+      </c>
+      <c r="W26" s="3">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="27" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="G27" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="H27" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="I27" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="J27" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="K27" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="L27" s="20" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="O27" s="20"/>
+      <c r="R27" s="3" t="str">
+        <v>C9</v>
+      </c>
+      <c r="S27" s="3">
+        <v>0</v>
+      </c>
+      <c r="T27" s="3">
+        <v>0</v>
+      </c>
+      <c r="U27" s="3">
+        <v>0</v>
+      </c>
+      <c r="V27" s="3">
+        <v>0</v>
+      </c>
+      <c r="W27" s="3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="28" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="G28" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="H28" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="I28" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="J28" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="K28" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="L28" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="O28" s="20"/>
+      <c r="R28" s="3" t="str">
+        <v>C10</v>
+      </c>
+      <c r="S28" s="3">
+        <v>0</v>
+      </c>
+      <c r="T28" s="3">
+        <v>0</v>
+      </c>
+      <c r="U28" s="3">
+        <v>0</v>
+      </c>
+      <c r="V28" s="3">
+        <v>0</v>
+      </c>
+      <c r="W28" s="3">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="29" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="G29" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="H29" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="I29" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="J29" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="K29" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="L29" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="O29" s="20"/>
+      <c r="R29" s="3" t="str">
+        <v>C11</v>
+      </c>
+      <c r="S29" s="3">
+        <v>0</v>
+      </c>
+      <c r="T29" s="3">
+        <v>0</v>
+      </c>
+      <c r="U29" s="3">
+        <v>0</v>
+      </c>
+      <c r="V29" s="3">
+        <v>0</v>
+      </c>
+      <c r="W29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="G30" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="H30" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="I30" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="J30" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="K30" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="L30" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="O30" s="20"/>
+      <c r="R30" s="3" t="str">
+        <v>C12</v>
+      </c>
+      <c r="S30" s="3">
+        <v>0</v>
+      </c>
+      <c r="T30" s="3">
+        <v>0</v>
+      </c>
+      <c r="U30" s="3">
+        <v>0</v>
+      </c>
+      <c r="V30" s="3">
+        <v>0</v>
+      </c>
+      <c r="W30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="G31" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="H31" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="I31" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="J31" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="K31" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="L31" s="3" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="O31" s="20"/>
+    </row>
+    <row r="32" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="O32" s="20"/>
+    </row>
+    <row r="33" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="O33" s="20"/>
+    </row>
+    <row r="34" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L34" s="36" cm="1">
+        <f t="array" ref="L34:L45">D3:D14 - _xlfn.BYROW(B3:B14, _xlfn.LAMBDA(_xlpm.r,SUM(_xlpm.r)))</f>
+        <v>120</v>
+      </c>
+      <c r="O34" s="20"/>
+      <c r="R34" s="3" t="str" cm="1">
+        <f t="array" ref="R34:W45">_xlfn.REDUCE(    B3:B14,
+            H3:H7,
+            _xlfn.LAMBDA(_xlpm.b,_xlpm.w,
+                _xlfn.HSTACK(
+                    _xlpm.b,
+                    _xlfn.DROP(
+                        _xlfn.REDUCE(
+                            _xlpm.w,
+                            D3:D14,
+                            _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.VSTACK(_xlpm.a, MIN(_xlfn.SINGLE(_xlpm.a) * 2 - SUM(_xlpm.a), _xlpm.v)))
+                        ),
+                        1
+                    )
+                )
+            )
+)</f>
+        <v>C1</v>
+      </c>
+      <c r="S34" s="3">
+        <v>120</v>
+      </c>
+      <c r="T34" s="3">
+        <v>50</v>
+      </c>
+      <c r="U34" s="3">
+        <v>112</v>
+      </c>
+      <c r="V34" s="3">
+        <v>120</v>
+      </c>
+      <c r="W34" s="3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L35" s="3">
+        <v>356</v>
+      </c>
+      <c r="O35" s="20"/>
+      <c r="R35" s="3" t="str">
+        <v>C2</v>
+      </c>
+      <c r="S35" s="3">
+        <v>356</v>
+      </c>
+      <c r="T35" s="3">
+        <v>0</v>
+      </c>
+      <c r="U35" s="3">
+        <v>0</v>
+      </c>
+      <c r="V35" s="3">
+        <v>356</v>
+      </c>
+      <c r="W35" s="3">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="36" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L36" s="3">
+        <v>312</v>
+      </c>
+      <c r="O36" s="20"/>
+      <c r="R36" s="3" t="str">
+        <v>C3</v>
+      </c>
+      <c r="S36" s="3">
+        <v>124</v>
+      </c>
+      <c r="T36" s="3">
+        <v>0</v>
+      </c>
+      <c r="U36" s="3">
+        <v>0</v>
+      </c>
+      <c r="V36" s="3">
+        <v>312</v>
+      </c>
+      <c r="W36" s="3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="37" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L37" s="3">
+        <v>437</v>
+      </c>
+      <c r="O37" s="20"/>
+      <c r="R37" s="3" t="str">
+        <v>C4</v>
+      </c>
+      <c r="S37" s="3">
+        <v>0</v>
+      </c>
+      <c r="T37" s="3">
+        <v>0</v>
+      </c>
+      <c r="U37" s="3">
+        <v>0</v>
+      </c>
+      <c r="V37" s="3">
+        <v>12</v>
+      </c>
+      <c r="W37" s="3">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="38" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L38" s="3">
+        <v>374</v>
+      </c>
+      <c r="O38" s="20"/>
+      <c r="R38" s="3" t="str">
+        <v>C5</v>
+      </c>
+      <c r="S38" s="3">
+        <v>0</v>
+      </c>
+      <c r="T38" s="3">
+        <v>0</v>
+      </c>
+      <c r="U38" s="3">
+        <v>0</v>
+      </c>
+      <c r="V38" s="3">
+        <v>0</v>
+      </c>
+      <c r="W38" s="3">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="39" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L39" s="3">
+        <v>258</v>
+      </c>
+      <c r="O39" s="20"/>
+      <c r="R39" s="3" t="str">
+        <v>C6</v>
+      </c>
+      <c r="S39" s="3">
+        <v>0</v>
+      </c>
+      <c r="T39" s="3">
+        <v>0</v>
+      </c>
+      <c r="U39" s="3">
+        <v>0</v>
+      </c>
+      <c r="V39" s="3">
+        <v>0</v>
+      </c>
+      <c r="W39" s="3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="40" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L40" s="3">
+        <v>369</v>
+      </c>
+      <c r="O40" s="20"/>
+      <c r="R40" s="3" t="str">
+        <v>C7</v>
+      </c>
+      <c r="S40" s="3">
+        <v>0</v>
+      </c>
+      <c r="T40" s="3">
+        <v>0</v>
+      </c>
+      <c r="U40" s="3">
+        <v>0</v>
+      </c>
+      <c r="V40" s="3">
+        <v>0</v>
+      </c>
+      <c r="W40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L41" s="3">
+        <v>418</v>
+      </c>
+      <c r="O41" s="20"/>
+      <c r="R41" s="3" t="str">
+        <v>C8</v>
+      </c>
+      <c r="S41" s="3">
+        <v>0</v>
+      </c>
+      <c r="T41" s="3">
+        <v>0</v>
+      </c>
+      <c r="U41" s="3">
+        <v>0</v>
+      </c>
+      <c r="V41" s="3">
+        <v>0</v>
+      </c>
+      <c r="W41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L42" s="3">
+        <v>308</v>
+      </c>
+      <c r="O42" s="20"/>
+      <c r="R42" s="3" t="str">
+        <v>C9</v>
+      </c>
+      <c r="S42" s="3">
+        <v>0</v>
+      </c>
+      <c r="T42" s="3">
+        <v>0</v>
+      </c>
+      <c r="U42" s="3">
+        <v>0</v>
+      </c>
+      <c r="V42" s="3">
+        <v>0</v>
+      </c>
+      <c r="W42" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L43" s="3">
+        <v>410</v>
+      </c>
+      <c r="O43" s="20"/>
+      <c r="R43" s="3" t="str">
+        <v>C10</v>
+      </c>
+      <c r="S43" s="3">
+        <v>0</v>
+      </c>
+      <c r="T43" s="3">
+        <v>0</v>
+      </c>
+      <c r="U43" s="3">
+        <v>0</v>
+      </c>
+      <c r="V43" s="3">
+        <v>0</v>
+      </c>
+      <c r="W43" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L44" s="3">
+        <v>491</v>
+      </c>
+      <c r="O44" s="20"/>
+      <c r="R44" s="3" t="str">
+        <v>C11</v>
+      </c>
+      <c r="S44" s="3">
+        <v>0</v>
+      </c>
+      <c r="T44" s="3">
+        <v>0</v>
+      </c>
+      <c r="U44" s="3">
+        <v>0</v>
+      </c>
+      <c r="V44" s="3">
+        <v>0</v>
+      </c>
+      <c r="W44" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L45" s="3">
+        <v>50</v>
+      </c>
+      <c r="O45" s="20"/>
+      <c r="R45" s="3" t="str">
+        <v>C12</v>
+      </c>
+      <c r="S45" s="3">
+        <v>0</v>
+      </c>
+      <c r="T45" s="3">
+        <v>0</v>
+      </c>
+      <c r="U45" s="3">
+        <v>0</v>
+      </c>
+      <c r="V45" s="3">
+        <v>0</v>
+      </c>
+      <c r="W45" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="O46" s="20"/>
+    </row>
+    <row r="47" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="O47" s="20"/>
+    </row>
+    <row r="48" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="O48" s="20"/>
+    </row>
+    <row r="49" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O49" s="20"/>
+    </row>
+    <row r="50" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O50" s="20"/>
+    </row>
+    <row r="51" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O51" s="20"/>
+    </row>
+    <row r="52" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O52" s="20"/>
+    </row>
+    <row r="53" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O53" s="20"/>
+    </row>
+    <row r="54" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O54" s="20"/>
+    </row>
+    <row r="55" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O55" s="20"/>
+    </row>
+    <row r="56" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O56" s="20"/>
+    </row>
+    <row r="57" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O57" s="20"/>
+    </row>
+    <row r="58" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O58" s="20"/>
+    </row>
+    <row r="59" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O59" s="20"/>
+    </row>
+    <row r="60" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O60" s="20"/>
+    </row>
+    <row r="61" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O61" s="20"/>
+    </row>
+    <row r="62" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O62" s="20"/>
+    </row>
+    <row r="63" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O63" s="20"/>
+    </row>
+    <row r="64" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O64" s="20"/>
+    </row>
+    <row r="65" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O65" s="20"/>
+    </row>
+    <row r="66" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O66" s="20"/>
+    </row>
+    <row r="67" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O67" s="20"/>
+    </row>
+    <row r="68" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O68" s="20"/>
+    </row>
+    <row r="69" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O69" s="20"/>
+    </row>
+    <row r="70" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O70" s="20"/>
+    </row>
+    <row r="71" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O71" s="20"/>
+    </row>
+    <row r="72" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O72" s="20"/>
+    </row>
+    <row r="73" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O73" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="K1:P1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Trying to find a way to breakdown Bo's solution
</commit_message>
<xml_diff>
--- a/CH-060 Match payments.xlsx
+++ b/CH-060 Match payments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F2A04B-9714-4D45-98FC-353F0A4FF428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DF11CF-CBAB-4BCE-ABA4-850E38EBEFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -212,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,6 +228,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,7 +438,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -533,16 +539,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1868,24 +1875,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="F1" s="38" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="F1" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="K1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="K1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
       <c r="R1" s="1" t="s">
         <v>25</v>
       </c>
@@ -2490,24 +2497,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:31" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="F1" s="38" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="F1" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="K1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="K1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
       <c r="AA1" s="1" t="s">
         <v>16</v>
       </c>
@@ -3279,7 +3286,7 @@
         <v>120</v>
       </c>
       <c r="G24" s="3" t="e">
-        <f>_xlfn.XLOOKUP(F24,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <f t="shared" ref="G24:G35" si="1">_xlfn.XLOOKUP(F24,$T$2:$T$6,$S$2:$S$6,,-1)</f>
         <v>#N/A</v>
       </c>
       <c r="L24" s="20"/>
@@ -3340,7 +3347,7 @@
         <v>356</v>
       </c>
       <c r="E25" s="3">
-        <f t="shared" ref="E25:E35" si="1">SUMIF($G$3:$G$7,"&lt;="&amp;C25,$H$3:$H$7)</f>
+        <f t="shared" ref="E25:E35" si="2">SUMIF($G$3:$G$7,"&lt;="&amp;C25,$H$3:$H$7)</f>
         <v>3362</v>
       </c>
       <c r="F25" s="36">
@@ -3348,7 +3355,7 @@
         <v>476</v>
       </c>
       <c r="G25" s="3" t="e">
-        <f>_xlfn.XLOOKUP(F25,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
       <c r="L25" s="20"/>
@@ -3394,7 +3401,7 @@
         <v>312</v>
       </c>
       <c r="E26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3362</v>
       </c>
       <c r="F26" s="36">
@@ -3402,7 +3409,7 @@
         <v>788</v>
       </c>
       <c r="G26" s="3" t="str">
-        <f>_xlfn.XLOOKUP(F26,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <f t="shared" si="1"/>
         <v>P3</v>
       </c>
       <c r="L26" s="20"/>
@@ -3448,7 +3455,7 @@
         <v>437</v>
       </c>
       <c r="E27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3362</v>
       </c>
       <c r="F27" s="36">
@@ -3456,7 +3463,7 @@
         <v>1225</v>
       </c>
       <c r="G27" s="3" t="str">
-        <f>_xlfn.XLOOKUP(F27,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <f t="shared" si="1"/>
         <v>P3</v>
       </c>
       <c r="L27" s="20"/>
@@ -3502,7 +3509,7 @@
         <v>374</v>
       </c>
       <c r="E28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3362</v>
       </c>
       <c r="F28" s="36">
@@ -3510,7 +3517,7 @@
         <v>1599</v>
       </c>
       <c r="G28" s="3" t="str">
-        <f>_xlfn.XLOOKUP(F28,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <f t="shared" si="1"/>
         <v>P4</v>
       </c>
       <c r="L28" s="20"/>
@@ -3556,7 +3563,7 @@
         <v>258</v>
       </c>
       <c r="E29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3362</v>
       </c>
       <c r="F29" s="36">
@@ -3564,7 +3571,7 @@
         <v>1857</v>
       </c>
       <c r="G29" s="3" t="str">
-        <f>_xlfn.XLOOKUP(F29,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <f t="shared" si="1"/>
         <v>P4</v>
       </c>
       <c r="L29" s="20"/>
@@ -3610,7 +3617,7 @@
         <v>369</v>
       </c>
       <c r="E30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3362</v>
       </c>
       <c r="F30" s="36">
@@ -3618,7 +3625,7 @@
         <v>2226</v>
       </c>
       <c r="G30" s="3" t="str">
-        <f>_xlfn.XLOOKUP(F30,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <f t="shared" si="1"/>
         <v>P4</v>
       </c>
       <c r="L30" s="20"/>
@@ -3664,7 +3671,7 @@
         <v>418</v>
       </c>
       <c r="E31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3362</v>
       </c>
       <c r="F31" s="36">
@@ -3672,7 +3679,7 @@
         <v>2644</v>
       </c>
       <c r="G31" s="3" t="str">
-        <f>_xlfn.XLOOKUP(F31,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <f t="shared" si="1"/>
         <v>P4</v>
       </c>
       <c r="L31" s="20"/>
@@ -3718,7 +3725,7 @@
         <v>308</v>
       </c>
       <c r="E32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3362</v>
       </c>
       <c r="F32" s="36">
@@ -3726,7 +3733,7 @@
         <v>2952</v>
       </c>
       <c r="G32" s="3" t="str">
-        <f>_xlfn.XLOOKUP(F32,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <f t="shared" si="1"/>
         <v>P4</v>
       </c>
       <c r="L32" s="20"/>
@@ -3772,7 +3779,7 @@
         <v>410</v>
       </c>
       <c r="E33" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3362</v>
       </c>
       <c r="F33" s="36">
@@ -3780,7 +3787,7 @@
         <v>3362</v>
       </c>
       <c r="G33" s="3" t="str">
-        <f>_xlfn.XLOOKUP(F33,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <f t="shared" si="1"/>
         <v>P5</v>
       </c>
       <c r="L33" s="20"/>
@@ -3826,7 +3833,7 @@
         <v>491</v>
       </c>
       <c r="E34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3362</v>
       </c>
       <c r="F34" s="36">
@@ -3834,7 +3841,7 @@
         <v>3853</v>
       </c>
       <c r="G34" s="3" t="str">
-        <f>_xlfn.XLOOKUP(F34,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <f t="shared" si="1"/>
         <v>P5</v>
       </c>
       <c r="N34" s="3" t="str">
@@ -3879,7 +3886,7 @@
         <v>50</v>
       </c>
       <c r="E35" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3362</v>
       </c>
       <c r="F35" s="36">
@@ -3887,7 +3894,7 @@
         <v>3903</v>
       </c>
       <c r="G35" s="3" t="str">
-        <f>_xlfn.XLOOKUP(F35,$T$2:$T$6,$S$2:$S$6,,-1)</f>
+        <f t="shared" si="1"/>
         <v>P5</v>
       </c>
       <c r="N35" s="3" t="str">
@@ -4090,24 +4097,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="F1" s="38" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="F1" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="K1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="K1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
       <c r="R1" s="37" t="s">
         <v>25</v>
       </c>
@@ -5200,24 +5207,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="F1" s="38" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="F1" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="K1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="K1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -5795,10 +5802,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D8F953-0749-4436-8A06-19D4F87E6D90}">
-  <dimension ref="B1:W73"/>
+  <dimension ref="A1:AJ73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q34" sqref="Q34"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19:W30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5821,30 +5828,30 @@
     <col min="23" max="16384" width="8.59765625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="38" t="s">
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="F1" s="38" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="F1" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="K1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="K1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
       <c r="R1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -5880,7 +5887,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
       <c r="B3" s="10" t="s">
         <v>4</v>
       </c>
@@ -5910,7 +5920,10 @@
       <c r="O3" s="14"/>
       <c r="P3" s="15"/>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
       <c r="B4" s="10" t="s">
         <v>5</v>
       </c>
@@ -5939,13 +5952,13 @@
       <c r="N4" s="33"/>
       <c r="O4" s="33"/>
       <c r="P4" s="34"/>
-      <c r="R4" s="40">
+      <c r="R4" s="38">
         <v>1</v>
       </c>
-      <c r="S4" s="40">
+      <c r="S4" s="38">
         <v>2</v>
       </c>
-      <c r="T4" s="40">
+      <c r="T4" s="38">
         <v>3</v>
       </c>
       <c r="V4" s="3" cm="1">
@@ -5953,7 +5966,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
       <c r="B5" s="10" t="s">
         <v>6</v>
       </c>
@@ -5988,20 +6004,23 @@
         <v>26</v>
       </c>
       <c r="P5" s="34"/>
-      <c r="R5" s="41">
+      <c r="R5" s="39">
         <v>4</v>
       </c>
-      <c r="S5" s="41">
+      <c r="S5" s="39">
         <v>5</v>
       </c>
-      <c r="T5" s="41">
+      <c r="T5" s="39">
         <v>6</v>
       </c>
       <c r="V5" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
       <c r="B6" s="10" t="s">
         <v>7</v>
       </c>
@@ -6030,20 +6049,43 @@
         <v>437</v>
       </c>
       <c r="P6" s="34"/>
-      <c r="R6" s="40">
+      <c r="R6" s="38">
         <v>7</v>
       </c>
-      <c r="S6" s="40">
+      <c r="S6" s="38">
         <v>8</v>
       </c>
-      <c r="T6" s="40">
+      <c r="T6" s="38">
         <v>9</v>
       </c>
       <c r="V6" s="3">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="AE6" s="36" cm="1">
+        <f t="array" ref="AE6:AE17">D3:D14</f>
+        <v>120</v>
+      </c>
+      <c r="AF6" s="3" cm="1">
+        <f t="array" ref="AF6:AF17">_xlfn.BYROW(L3:L14,_xlfn.LAMBDA(_xlpm.r,SUM(_xlpm.r)))</f>
+        <v>120</v>
+      </c>
+      <c r="AG6" s="36">
+        <f>AE6-AF6</f>
+        <v>0</v>
+      </c>
+      <c r="AI6" s="36" cm="1">
+        <f t="array" ref="AI6:AI17">_xlfn.ANCHORARRAY(AE6)</f>
+        <v>120</v>
+      </c>
+      <c r="AJ6" s="36" cm="1">
+        <f t="array" ref="AJ6:AJ17">AI6:AI17-_xlfn.BYROW(AF6:AG17,_xlfn.LAMBDA(_xlpm.r,SUM(_xlpm.r)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
       <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
@@ -6074,11 +6116,30 @@
       <c r="P7" s="34">
         <v>37</v>
       </c>
-      <c r="R7" s="40"/>
-      <c r="S7" s="40"/>
-      <c r="T7" s="40"/>
-    </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="R7" s="38"/>
+      <c r="S7" s="38"/>
+      <c r="T7" s="38"/>
+      <c r="AE7" s="3">
+        <v>356</v>
+      </c>
+      <c r="AF7" s="3">
+        <v>356</v>
+      </c>
+      <c r="AG7" s="36">
+        <f t="shared" ref="AG7:AG17" si="0">AE7-AF7</f>
+        <v>0</v>
+      </c>
+      <c r="AI7" s="3">
+        <v>356</v>
+      </c>
+      <c r="AJ7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
       <c r="B8" s="10" t="s">
         <v>9</v>
       </c>
@@ -6098,8 +6159,27 @@
       <c r="P8" s="34">
         <v>258</v>
       </c>
-    </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="AE8" s="3">
+        <v>312</v>
+      </c>
+      <c r="AF8" s="3">
+        <v>124</v>
+      </c>
+      <c r="AG8" s="36">
+        <f t="shared" si="0"/>
+        <v>188</v>
+      </c>
+      <c r="AI8" s="3">
+        <v>312</v>
+      </c>
+      <c r="AJ8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
       <c r="B9" s="10" t="s">
         <v>10</v>
       </c>
@@ -6119,8 +6199,27 @@
       <c r="P9" s="34">
         <v>369</v>
       </c>
-    </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="AE9" s="3">
+        <v>437</v>
+      </c>
+      <c r="AF9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="36">
+        <f t="shared" si="0"/>
+        <v>437</v>
+      </c>
+      <c r="AI9" s="3">
+        <v>437</v>
+      </c>
+      <c r="AJ9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
       <c r="B10" s="10" t="s">
         <v>11</v>
       </c>
@@ -6140,8 +6239,27 @@
       <c r="P10" s="34">
         <v>418</v>
       </c>
-    </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="AE10" s="3">
+        <v>374</v>
+      </c>
+      <c r="AF10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="36">
+        <f t="shared" si="0"/>
+        <v>374</v>
+      </c>
+      <c r="AI10" s="3">
+        <v>374</v>
+      </c>
+      <c r="AJ10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
       <c r="B11" s="10" t="s">
         <v>12</v>
       </c>
@@ -6161,8 +6279,27 @@
       <c r="P11" s="34">
         <v>308</v>
       </c>
-    </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="AE11" s="3">
+        <v>258</v>
+      </c>
+      <c r="AF11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="36">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="AI11" s="3">
+        <v>258</v>
+      </c>
+      <c r="AJ11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
       <c r="B12" s="10" t="s">
         <v>13</v>
       </c>
@@ -6183,8 +6320,27 @@
       <c r="P12" s="34">
         <v>410</v>
       </c>
-    </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="AE12" s="3">
+        <v>369</v>
+      </c>
+      <c r="AF12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="36">
+        <f t="shared" si="0"/>
+        <v>369</v>
+      </c>
+      <c r="AI12" s="3">
+        <v>369</v>
+      </c>
+      <c r="AJ12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
       <c r="B13" s="10" t="s">
         <v>14</v>
       </c>
@@ -6213,8 +6369,27 @@
       <c r="P13" s="15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="AE13" s="3">
+        <v>418</v>
+      </c>
+      <c r="AF13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="36">
+        <f t="shared" si="0"/>
+        <v>418</v>
+      </c>
+      <c r="AI13" s="3">
+        <v>418</v>
+      </c>
+      <c r="AJ13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
       <c r="B14" s="10" t="s">
         <v>22</v>
       </c>
@@ -6243,33 +6418,97 @@
       <c r="P14" s="26" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="AE14" s="3">
+        <v>308</v>
+      </c>
+      <c r="AF14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="36">
+        <f t="shared" si="0"/>
+        <v>308</v>
+      </c>
+      <c r="AI14" s="3">
+        <v>308</v>
+      </c>
+      <c r="AJ14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="G15" s="20"/>
       <c r="L15" s="27"/>
       <c r="O15" s="20"/>
-    </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="AE15" s="3">
+        <v>410</v>
+      </c>
+      <c r="AF15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="36">
+        <f t="shared" si="0"/>
+        <v>410</v>
+      </c>
+      <c r="AI15" s="3">
+        <v>410</v>
+      </c>
+      <c r="AJ15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="G16" s="20"/>
       <c r="L16" s="27"/>
       <c r="O16" s="20"/>
       <c r="R16" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="AE16" s="3">
+        <v>491</v>
+      </c>
+      <c r="AF16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="36">
+        <f t="shared" si="0"/>
+        <v>491</v>
+      </c>
+      <c r="AI16" s="3">
+        <v>491</v>
+      </c>
+      <c r="AJ16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="7:36" x14ac:dyDescent="0.25">
       <c r="G17" s="20"/>
       <c r="L17" s="27"/>
       <c r="O17" s="20"/>
-    </row>
-    <row r="18" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="AE17" s="3">
+        <v>50</v>
+      </c>
+      <c r="AF17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="36">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="AI17" s="3">
+        <v>50</v>
+      </c>
+      <c r="AJ17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="7:36" x14ac:dyDescent="0.25">
       <c r="G18" s="20"/>
       <c r="L18" s="27"/>
       <c r="O18" s="20"/>
     </row>
-    <row r="19" spans="7:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:36" x14ac:dyDescent="0.25">
       <c r="G19" s="3" t="str" cm="1">
         <f t="array" ref="G19:L31">_xlfn.LET(
     _xlpm.d, _xlfn.DROP(
@@ -6317,7 +6556,7 @@
 _xlfn.VSTACK(_xlfn.TOROW(F2:F7),IF(_xlfn.BYROW(_xlpm.d,SUM)+(_xlpm.d&gt;""),_xlpm.d,"NP")))</f>
         <v>#NAME?</v>
       </c>
-      <c r="R19" s="3" t="str" cm="1">
+      <c r="R19" s="42" t="str" cm="1">
         <f t="array" ref="R19:W30">_xlfn.REDUCE(    B3:B14,
             H3:H7,
             _xlfn.LAMBDA(_xlpm.b,_xlpm.w,
@@ -6336,23 +6575,57 @@
 )</f>
         <v>C1</v>
       </c>
-      <c r="S19" s="3">
+      <c r="S19" s="42">
         <v>120</v>
       </c>
-      <c r="T19" s="3">
-        <v>0</v>
-      </c>
-      <c r="U19" s="3">
-        <v>0</v>
-      </c>
-      <c r="V19" s="3">
-        <v>0</v>
-      </c>
-      <c r="W19" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="T19" s="42">
+        <v>0</v>
+      </c>
+      <c r="U19" s="42">
+        <v>0</v>
+      </c>
+      <c r="V19" s="42">
+        <v>0</v>
+      </c>
+      <c r="W19" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="3" cm="1">
+        <f t="array" ref="Y19:AD30">_xlfn.REDUCE(    A3:A14,
+            H3:H7,
+            _xlfn.LAMBDA(_xlpm.b,_xlpm.w,
+                _xlfn.HSTACK(
+                    _xlpm.b,
+                    _xlfn.DROP(
+                        _xlfn.REDUCE(
+                            _xlpm.w,
+                            D3:D14 - _xlfn.BYROW(_xlpm.b, _xlfn.LAMBDA(_xlpm.r,SUM(_xlpm.r))),
+                            _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.VSTACK(_xlpm.a, _xlpm.v))
+                        ),
+                        1
+                    )
+                )
+            )
+)</f>
+        <v>1</v>
+      </c>
+      <c r="Z19" s="3">
+        <v>119</v>
+      </c>
+      <c r="AA19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="7:36" x14ac:dyDescent="0.25">
       <c r="G20" s="3" t="e">
         <v>#NAME?</v>
       </c>
@@ -6372,26 +6645,44 @@
         <v>#NAME?</v>
       </c>
       <c r="O20" s="20"/>
-      <c r="R20" s="3" t="str">
+      <c r="R20" s="42" t="str">
         <v>C2</v>
       </c>
-      <c r="S20" s="3">
+      <c r="S20" s="42">
         <v>356</v>
       </c>
-      <c r="T20" s="3">
-        <v>0</v>
-      </c>
-      <c r="U20" s="3">
-        <v>0</v>
-      </c>
-      <c r="V20" s="3">
-        <v>0</v>
-      </c>
-      <c r="W20" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="T20" s="42">
+        <v>0</v>
+      </c>
+      <c r="U20" s="42">
+        <v>0</v>
+      </c>
+      <c r="V20" s="42">
+        <v>0</v>
+      </c>
+      <c r="W20" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>2</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>354</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="7:36" x14ac:dyDescent="0.25">
       <c r="G21" s="3" t="e">
         <v>#NAME?</v>
       </c>
@@ -6411,26 +6702,44 @@
         <v>#NAME?</v>
       </c>
       <c r="O21" s="20"/>
-      <c r="R21" s="3" t="str">
+      <c r="R21" s="42" t="str">
         <v>C3</v>
       </c>
-      <c r="S21" s="3">
+      <c r="S21" s="42">
         <v>124</v>
       </c>
-      <c r="T21" s="3">
+      <c r="T21" s="42">
         <v>50</v>
       </c>
-      <c r="U21" s="3">
+      <c r="U21" s="42">
         <v>112</v>
       </c>
-      <c r="V21" s="3">
+      <c r="V21" s="42">
         <v>26</v>
       </c>
-      <c r="W21" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="W21" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="3">
+        <v>3</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>309</v>
+      </c>
+      <c r="AA21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="7:36" x14ac:dyDescent="0.25">
       <c r="G22" s="3" t="e">
         <v>#NAME?</v>
       </c>
@@ -6450,26 +6759,44 @@
         <v>#NAME?</v>
       </c>
       <c r="O22" s="20"/>
-      <c r="R22" s="3" t="str">
+      <c r="R22" s="42" t="str">
         <v>C4</v>
       </c>
-      <c r="S22" s="3">
-        <v>0</v>
-      </c>
-      <c r="T22" s="3">
-        <v>0</v>
-      </c>
-      <c r="U22" s="3">
-        <v>0</v>
-      </c>
-      <c r="V22" s="3">
+      <c r="S22" s="42">
+        <v>0</v>
+      </c>
+      <c r="T22" s="42">
+        <v>0</v>
+      </c>
+      <c r="U22" s="42">
+        <v>0</v>
+      </c>
+      <c r="V22" s="42">
         <v>437</v>
       </c>
-      <c r="W22" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="W22" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>433</v>
+      </c>
+      <c r="AA22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="7:36" x14ac:dyDescent="0.25">
       <c r="G23" s="3" t="e">
         <v>#NAME?</v>
       </c>
@@ -6489,26 +6816,44 @@
         <v>#NAME?</v>
       </c>
       <c r="O23" s="20"/>
-      <c r="R23" s="3" t="str">
+      <c r="R23" s="42" t="str">
         <v>C5</v>
       </c>
-      <c r="S23" s="3">
-        <v>0</v>
-      </c>
-      <c r="T23" s="3">
-        <v>0</v>
-      </c>
-      <c r="U23" s="3">
-        <v>0</v>
-      </c>
-      <c r="V23" s="3">
+      <c r="S23" s="42">
+        <v>0</v>
+      </c>
+      <c r="T23" s="42">
+        <v>0</v>
+      </c>
+      <c r="U23" s="42">
+        <v>0</v>
+      </c>
+      <c r="V23" s="42">
         <v>337</v>
       </c>
-      <c r="W23" s="3">
+      <c r="W23" s="42">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="Y23" s="3">
+        <v>5</v>
+      </c>
+      <c r="Z23" s="3">
+        <v>369</v>
+      </c>
+      <c r="AA23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="7:36" x14ac:dyDescent="0.25">
       <c r="G24" s="3" t="e">
         <v>#NAME?</v>
       </c>
@@ -6528,26 +6873,44 @@
         <v>#NAME?</v>
       </c>
       <c r="O24" s="20"/>
-      <c r="R24" s="3" t="str">
+      <c r="R24" s="42" t="str">
         <v>C6</v>
       </c>
-      <c r="S24" s="3">
-        <v>0</v>
-      </c>
-      <c r="T24" s="3">
-        <v>0</v>
-      </c>
-      <c r="U24" s="3">
-        <v>0</v>
-      </c>
-      <c r="V24" s="3">
-        <v>0</v>
-      </c>
-      <c r="W24" s="3">
+      <c r="S24" s="42">
+        <v>0</v>
+      </c>
+      <c r="T24" s="42">
+        <v>0</v>
+      </c>
+      <c r="U24" s="42">
+        <v>0</v>
+      </c>
+      <c r="V24" s="42">
+        <v>0</v>
+      </c>
+      <c r="W24" s="42">
         <v>258</v>
       </c>
-    </row>
-    <row r="25" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="Y24" s="3">
+        <v>6</v>
+      </c>
+      <c r="Z24" s="3">
+        <v>252</v>
+      </c>
+      <c r="AA24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="7:36" x14ac:dyDescent="0.25">
       <c r="G25" s="3" t="e">
         <v>#NAME?</v>
       </c>
@@ -6567,26 +6930,44 @@
         <v>#NAME?</v>
       </c>
       <c r="O25" s="20"/>
-      <c r="R25" s="3" t="str">
+      <c r="R25" s="42" t="str">
         <v>C7</v>
       </c>
-      <c r="S25" s="3">
-        <v>0</v>
-      </c>
-      <c r="T25" s="3">
-        <v>0</v>
-      </c>
-      <c r="U25" s="3">
-        <v>0</v>
-      </c>
-      <c r="V25" s="3">
-        <v>0</v>
-      </c>
-      <c r="W25" s="3">
+      <c r="S25" s="42">
+        <v>0</v>
+      </c>
+      <c r="T25" s="42">
+        <v>0</v>
+      </c>
+      <c r="U25" s="42">
+        <v>0</v>
+      </c>
+      <c r="V25" s="42">
+        <v>0</v>
+      </c>
+      <c r="W25" s="42">
         <v>369</v>
       </c>
-    </row>
-    <row r="26" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="Y25" s="3">
+        <v>7</v>
+      </c>
+      <c r="Z25" s="3">
+        <v>362</v>
+      </c>
+      <c r="AA25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="7:36" x14ac:dyDescent="0.25">
       <c r="G26" s="3" t="e">
         <v>#NAME?</v>
       </c>
@@ -6606,26 +6987,44 @@
         <v>#NAME?</v>
       </c>
       <c r="O26" s="20"/>
-      <c r="R26" s="3" t="str">
+      <c r="R26" s="42" t="str">
         <v>C8</v>
       </c>
-      <c r="S26" s="3">
-        <v>0</v>
-      </c>
-      <c r="T26" s="3">
-        <v>0</v>
-      </c>
-      <c r="U26" s="3">
-        <v>0</v>
-      </c>
-      <c r="V26" s="3">
-        <v>0</v>
-      </c>
-      <c r="W26" s="3">
+      <c r="S26" s="42">
+        <v>0</v>
+      </c>
+      <c r="T26" s="42">
+        <v>0</v>
+      </c>
+      <c r="U26" s="42">
+        <v>0</v>
+      </c>
+      <c r="V26" s="42">
+        <v>0</v>
+      </c>
+      <c r="W26" s="42">
         <v>418</v>
       </c>
-    </row>
-    <row r="27" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="Y26" s="3">
+        <v>8</v>
+      </c>
+      <c r="Z26" s="3">
+        <v>410</v>
+      </c>
+      <c r="AA26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="7:36" x14ac:dyDescent="0.25">
       <c r="G27" s="3" t="e">
         <v>#NAME?</v>
       </c>
@@ -6645,26 +7044,44 @@
         <v>#NAME?</v>
       </c>
       <c r="O27" s="20"/>
-      <c r="R27" s="3" t="str">
+      <c r="R27" s="42" t="str">
         <v>C9</v>
       </c>
-      <c r="S27" s="3">
-        <v>0</v>
-      </c>
-      <c r="T27" s="3">
-        <v>0</v>
-      </c>
-      <c r="U27" s="3">
-        <v>0</v>
-      </c>
-      <c r="V27" s="3">
-        <v>0</v>
-      </c>
-      <c r="W27" s="3">
+      <c r="S27" s="42">
+        <v>0</v>
+      </c>
+      <c r="T27" s="42">
+        <v>0</v>
+      </c>
+      <c r="U27" s="42">
+        <v>0</v>
+      </c>
+      <c r="V27" s="42">
+        <v>0</v>
+      </c>
+      <c r="W27" s="42">
         <v>308</v>
       </c>
-    </row>
-    <row r="28" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="Y27" s="3">
+        <v>9</v>
+      </c>
+      <c r="Z27" s="3">
+        <v>299</v>
+      </c>
+      <c r="AA27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="7:36" x14ac:dyDescent="0.25">
       <c r="G28" s="3" t="e">
         <v>#NAME?</v>
       </c>
@@ -6684,26 +7101,44 @@
         <v>#NAME?</v>
       </c>
       <c r="O28" s="20"/>
-      <c r="R28" s="3" t="str">
+      <c r="R28" s="42" t="str">
         <v>C10</v>
       </c>
-      <c r="S28" s="3">
-        <v>0</v>
-      </c>
-      <c r="T28" s="3">
-        <v>0</v>
-      </c>
-      <c r="U28" s="3">
-        <v>0</v>
-      </c>
-      <c r="V28" s="3">
-        <v>0</v>
-      </c>
-      <c r="W28" s="3">
+      <c r="S28" s="42">
+        <v>0</v>
+      </c>
+      <c r="T28" s="42">
+        <v>0</v>
+      </c>
+      <c r="U28" s="42">
+        <v>0</v>
+      </c>
+      <c r="V28" s="42">
+        <v>0</v>
+      </c>
+      <c r="W28" s="42">
         <v>410</v>
       </c>
-    </row>
-    <row r="29" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="Y28" s="3">
+        <v>10</v>
+      </c>
+      <c r="Z28" s="3">
+        <v>400</v>
+      </c>
+      <c r="AA28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="7:36" x14ac:dyDescent="0.25">
       <c r="G29" s="3" t="e">
         <v>#NAME?</v>
       </c>
@@ -6723,26 +7158,44 @@
         <v>#NAME?</v>
       </c>
       <c r="O29" s="20"/>
-      <c r="R29" s="3" t="str">
+      <c r="R29" s="42" t="str">
         <v>C11</v>
       </c>
-      <c r="S29" s="3">
-        <v>0</v>
-      </c>
-      <c r="T29" s="3">
-        <v>0</v>
-      </c>
-      <c r="U29" s="3">
-        <v>0</v>
-      </c>
-      <c r="V29" s="3">
-        <v>0</v>
-      </c>
-      <c r="W29" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="S29" s="42">
+        <v>0</v>
+      </c>
+      <c r="T29" s="42">
+        <v>0</v>
+      </c>
+      <c r="U29" s="42">
+        <v>0</v>
+      </c>
+      <c r="V29" s="42">
+        <v>0</v>
+      </c>
+      <c r="W29" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="3">
+        <v>11</v>
+      </c>
+      <c r="Z29" s="3">
+        <v>480</v>
+      </c>
+      <c r="AA29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="7:36" x14ac:dyDescent="0.25">
       <c r="G30" s="3" t="e">
         <v>#NAME?</v>
       </c>
@@ -6762,26 +7215,44 @@
         <v>#NAME?</v>
       </c>
       <c r="O30" s="20"/>
-      <c r="R30" s="3" t="str">
+      <c r="R30" s="42" t="str">
         <v>C12</v>
       </c>
-      <c r="S30" s="3">
-        <v>0</v>
-      </c>
-      <c r="T30" s="3">
-        <v>0</v>
-      </c>
-      <c r="U30" s="3">
-        <v>0</v>
-      </c>
-      <c r="V30" s="3">
-        <v>0</v>
-      </c>
-      <c r="W30" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="S30" s="42">
+        <v>0</v>
+      </c>
+      <c r="T30" s="42">
+        <v>0</v>
+      </c>
+      <c r="U30" s="42">
+        <v>0</v>
+      </c>
+      <c r="V30" s="42">
+        <v>0</v>
+      </c>
+      <c r="W30" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="3">
+        <v>12</v>
+      </c>
+      <c r="Z30" s="3">
+        <v>38</v>
+      </c>
+      <c r="AA30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="7:36" x14ac:dyDescent="0.25">
       <c r="G31" s="3" t="e">
         <v>#NAME?</v>
       </c>
@@ -6802,7 +7273,7 @@
       </c>
       <c r="O31" s="20"/>
     </row>
-    <row r="32" spans="7:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="7:36" x14ac:dyDescent="0.25">
       <c r="O32" s="20"/>
     </row>
     <row r="33" spans="12:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Hit another wall on understanding Bo's solution
</commit_message>
<xml_diff>
--- a/CH-060 Match payments.xlsx
+++ b/CH-060 Match payments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DF11CF-CBAB-4BCE-ABA4-850E38EBEFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6668F7-480C-4C64-922B-8D250C0BEB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,6 +28,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Alternate3!$B$2:$B$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$B$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$B$15</definedName>
+    <definedName name="_na">Alternate3!$E$48:$E$51</definedName>
     <definedName name="allocate_payment">_xlfn.LAMBDA(_xlpm.costs,_xlpm.payments,_xlpm.allocations,_xlpm.position, _xlfn.LET(_xlpm._costRows, ROWS(_xlpm.costs), _xlpm._paymentColumns, COLUMNS(_xlpm.payments), _xlpm._seq, _xlfn.WRAPCOLS(_xlfn.SEQUENCE(_xlpm._costRows * _xlpm._paymentColumns), _xlpm._costRows), _xlpm._col, INT((_xlpm.position - 1) / _xlpm._costRows) + 1, _xlpm._row, MOD(_xlpm.position - 1, _xlpm._costRows) + 1, _xlpm._cost, INDEX(_xlpm.costs, _xlpm._row, 1), _xlpm._payment, INDEX(_xlpm.payments, 1, _xlpm._col), _xlpm._newAllocation, IF(_xlpm._cost &lt;= _xlpm._payment, _xlpm._cost, _xlpm._payment), _xlpm._newAllocations, IF(_xlpm._seq = _xlpm.position, _xlpm._newAllocation, 0) + _xlpm.allocations, _xlpm._newTotal, _xlfn.LAMBDA(_xlpm.seq,_xlpm.pos,_xlpm.arr, IF(_xlpm.seq = _xlpm.pos, _xlpm.arr - _xlpm._newAllocation, _xlpm.arr)), _xlpm._newCosts, _xlpm._newTotal(_xlfn.SEQUENCE(_xlpm._costRows), _xlpm._row, _xlpm.costs), _xlpm._newPayments, _xlpm._newTotal(_xlfn.SEQUENCE(, _xlpm._paymentColumns), _xlpm._col, _xlpm.payments), IF((_xlpm.position + 1) &gt; MAX(_xlpm._seq), _xlpm._newAllocations, allocate_payment(_xlpm._newCosts, _xlpm._newPayments, _xlpm._newAllocations, _xlpm.position + 1))))</definedName>
     <definedName name="allocate_payments_usage">_xlfn.LET(_xlpm.costs, [1]Sheet1!B1048560:B1048571, _xlpm.payments, _xlfn.TOROW([1]Sheet1!F1048560:F1048564), _xlpm.empty_array, _xlfn.MAKEARRAY(ROWS(_xlpm.costs), COLUMNS(_xlpm.payments), _xlfn.LAMBDA(_xlpm.r,_xlpm.c, 0)), _xlpm.header, _xlfn.HSTACK("", _xlfn.TOROW([1]Sheet1!D1048560:D1048564)), _xlfn.VSTACK(_xlpm.header, _xlfn.HSTACK([1]Sheet1!XFD1048560:XFD1048571, allocate_payment(_xlpm.costs, _xlpm.payments, _xlpm.empty_array, 1))))</definedName>
     <definedName name="Trial.allocate_payment">_xlfn.LAMBDA(_xlpm.costs,_xlpm.payments,_xlpm.allocations,_xlpm.position, _xlfn.LET(_xlpm._costRows, ROWS(_xlpm.costs), _xlpm._paymentColumns, COLUMNS(_xlpm.payments), _xlpm._seq, _xlfn.WRAPCOLS(_xlfn.SEQUENCE(_xlpm._costRows * _xlpm._paymentColumns), _xlpm._costRows), _xlpm._col, INT((_xlpm.position - 1) / _xlpm._costRows) + 1, _xlpm._row, MOD(_xlpm.position - 1, _xlpm._costRows) + 1, _xlpm._cost, INDEX(_xlpm.costs, _xlpm._row, 1), _xlpm._payment, INDEX(_xlpm.payments, 1, _xlpm._col), _xlpm._newAllocation, IF(_xlpm._cost &lt;= _xlpm._payment, _xlpm._cost, _xlpm._payment), _xlpm._newAllocations, IF(_xlpm._seq = _xlpm.position, _xlpm._newAllocation, 0) + _xlpm.allocations, _xlpm._newTotal, _xlfn.LAMBDA(_xlpm.seq,_xlpm.pos,_xlpm.arr, IF(_xlpm.seq = _xlpm.pos, _xlpm.arr - _xlpm._newAllocation, _xlpm.arr)), _xlpm._newCosts, _xlpm._newTotal(_xlfn.SEQUENCE(_xlpm._costRows), _xlpm._row, _xlpm.costs), _xlpm._newPayments, _xlpm._newTotal(_xlfn.SEQUENCE(, _xlpm._paymentColumns), _xlpm._col, _xlpm.payments), IF((_xlpm.position + 1) &gt; MAX(_xlpm._seq), _xlpm._newAllocations, Trial.allocate_payment(_xlpm._newCosts, _xlpm._newPayments, _xlpm._newAllocations, _xlpm.position + 1))))</definedName>
@@ -543,13 +544,13 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1540,6 +1541,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>510978</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>109243</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="A white background with black text&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2327683A-49DD-1D96-051C-3C401B41A24F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6994071" y="8776607"/>
+          <a:ext cx="5096586" cy="2762636"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -1821,7 +1871,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="715" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="723" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1875,24 +1925,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="F1" s="40" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="F1" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="K1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="K1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
       <c r="R1" s="1" t="s">
         <v>25</v>
       </c>
@@ -2497,24 +2547,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:31" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="F1" s="40" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="F1" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="K1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="K1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
       <c r="AA1" s="1" t="s">
         <v>16</v>
       </c>
@@ -4097,24 +4147,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="F1" s="40" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="F1" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="K1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="K1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
       <c r="R1" s="37" t="s">
         <v>25</v>
       </c>
@@ -5207,24 +5257,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="F1" s="40" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="F1" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="K1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="K1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -5802,10 +5852,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D8F953-0749-4436-8A06-19D4F87E6D90}">
-  <dimension ref="A1:AJ73"/>
+  <dimension ref="A1:AJ72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19:W30"/>
+      <selection activeCell="W51" sqref="W51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5825,28 +5875,30 @@
     <col min="13" max="16" width="6" style="3" customWidth="1"/>
     <col min="17" max="21" width="8.59765625" style="3"/>
     <col min="22" max="22" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.59765625" style="3"/>
+    <col min="23" max="25" width="8.59765625" style="3"/>
+    <col min="26" max="26" width="8.796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="8.59765625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="F1" s="40" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="F1" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="K1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="K1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
       <c r="R1" s="1" t="s">
         <v>25</v>
       </c>
@@ -6521,7 +6573,7 @@
                     _xlfn.DROP(
                         _xlfn.REDUCE(
                             _xlpm.w,
-                            D3:D14 - _xlfn.BYROW(D3:D14, _xlfn.LAMBDA(_xlpm.r,SUM(_xlpm.r))),
+                            D3:D14 - _xlfn.BYROW(_xlpm.b, _xlfn.LAMBDA(_xlpm.r,SUM(_xlpm.r))),
                             _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.VSTACK(_xlpm.a, MIN(_xlfn.SINGLE(_xlpm.a) * 2 - SUM(_xlpm.a), _xlpm.v)))
                         ),
                         1
@@ -6556,7 +6608,7 @@
 _xlfn.VSTACK(_xlfn.TOROW(F2:F7),IF(_xlfn.BYROW(_xlpm.d,SUM)+(_xlpm.d&gt;""),_xlpm.d,"NP")))</f>
         <v>#NAME?</v>
       </c>
-      <c r="R19" s="42" t="str" cm="1">
+      <c r="R19" s="40" t="str" cm="1">
         <f t="array" ref="R19:W30">_xlfn.REDUCE(    B3:B14,
             H3:H7,
             _xlfn.LAMBDA(_xlpm.b,_xlpm.w,
@@ -6575,23 +6627,23 @@
 )</f>
         <v>C1</v>
       </c>
-      <c r="S19" s="42">
+      <c r="S19" s="40">
         <v>120</v>
       </c>
-      <c r="T19" s="42">
-        <v>0</v>
-      </c>
-      <c r="U19" s="42">
-        <v>0</v>
-      </c>
-      <c r="V19" s="42">
-        <v>0</v>
-      </c>
-      <c r="W19" s="42">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="3" cm="1">
-        <f t="array" ref="Y19:AD30">_xlfn.REDUCE(    A3:A14,
+      <c r="T19" s="40">
+        <v>0</v>
+      </c>
+      <c r="U19" s="40">
+        <v>0</v>
+      </c>
+      <c r="V19" s="40">
+        <v>0</v>
+      </c>
+      <c r="W19" s="40">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="3" t="str" cm="1">
+        <f t="array" ref="Y19:AD30">_xlfn.REDUCE(    B3:B14,
             H3:H7,
             _xlfn.LAMBDA(_xlpm.b,_xlpm.w,
                 _xlfn.HSTACK(
@@ -6607,10 +6659,10 @@
                 )
             )
 )</f>
-        <v>1</v>
+        <v>C1</v>
       </c>
       <c r="Z19" s="3">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AA19" s="3">
         <v>0</v>
@@ -6645,29 +6697,29 @@
         <v>#NAME?</v>
       </c>
       <c r="O20" s="20"/>
-      <c r="R20" s="42" t="str">
+      <c r="R20" s="40" t="str">
         <v>C2</v>
       </c>
-      <c r="S20" s="42">
+      <c r="S20" s="40">
         <v>356</v>
       </c>
-      <c r="T20" s="42">
-        <v>0</v>
-      </c>
-      <c r="U20" s="42">
-        <v>0</v>
-      </c>
-      <c r="V20" s="42">
-        <v>0</v>
-      </c>
-      <c r="W20" s="42">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="3">
-        <v>2</v>
+      <c r="T20" s="40">
+        <v>0</v>
+      </c>
+      <c r="U20" s="40">
+        <v>0</v>
+      </c>
+      <c r="V20" s="40">
+        <v>0</v>
+      </c>
+      <c r="W20" s="40">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="3" t="str">
+        <v>C2</v>
       </c>
       <c r="Z20" s="3">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="AA20" s="3">
         <v>0</v>
@@ -6702,29 +6754,29 @@
         <v>#NAME?</v>
       </c>
       <c r="O21" s="20"/>
-      <c r="R21" s="42" t="str">
+      <c r="R21" s="40" t="str">
         <v>C3</v>
       </c>
-      <c r="S21" s="42">
+      <c r="S21" s="40">
         <v>124</v>
       </c>
-      <c r="T21" s="42">
+      <c r="T21" s="40">
         <v>50</v>
       </c>
-      <c r="U21" s="42">
+      <c r="U21" s="40">
         <v>112</v>
       </c>
-      <c r="V21" s="42">
+      <c r="V21" s="40">
         <v>26</v>
       </c>
-      <c r="W21" s="42">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="3">
-        <v>3</v>
+      <c r="W21" s="40">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="3" t="str">
+        <v>C3</v>
       </c>
       <c r="Z21" s="3">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="AA21" s="3">
         <v>0</v>
@@ -6759,29 +6811,29 @@
         <v>#NAME?</v>
       </c>
       <c r="O22" s="20"/>
-      <c r="R22" s="42" t="str">
+      <c r="R22" s="40" t="str">
         <v>C4</v>
       </c>
-      <c r="S22" s="42">
-        <v>0</v>
-      </c>
-      <c r="T22" s="42">
-        <v>0</v>
-      </c>
-      <c r="U22" s="42">
-        <v>0</v>
-      </c>
-      <c r="V22" s="42">
+      <c r="S22" s="40">
+        <v>0</v>
+      </c>
+      <c r="T22" s="40">
+        <v>0</v>
+      </c>
+      <c r="U22" s="40">
+        <v>0</v>
+      </c>
+      <c r="V22" s="40">
         <v>437</v>
       </c>
-      <c r="W22" s="42">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="3">
-        <v>4</v>
+      <c r="W22" s="40">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="3" t="str">
+        <v>C4</v>
       </c>
       <c r="Z22" s="3">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="AA22" s="3">
         <v>0</v>
@@ -6816,29 +6868,29 @@
         <v>#NAME?</v>
       </c>
       <c r="O23" s="20"/>
-      <c r="R23" s="42" t="str">
+      <c r="R23" s="40" t="str">
         <v>C5</v>
       </c>
-      <c r="S23" s="42">
-        <v>0</v>
-      </c>
-      <c r="T23" s="42">
-        <v>0</v>
-      </c>
-      <c r="U23" s="42">
-        <v>0</v>
-      </c>
-      <c r="V23" s="42">
+      <c r="S23" s="40">
+        <v>0</v>
+      </c>
+      <c r="T23" s="40">
+        <v>0</v>
+      </c>
+      <c r="U23" s="40">
+        <v>0</v>
+      </c>
+      <c r="V23" s="40">
         <v>337</v>
       </c>
-      <c r="W23" s="42">
+      <c r="W23" s="40">
         <v>37</v>
       </c>
-      <c r="Y23" s="3">
-        <v>5</v>
+      <c r="Y23" s="3" t="str">
+        <v>C5</v>
       </c>
       <c r="Z23" s="3">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="AA23" s="3">
         <v>0</v>
@@ -6873,29 +6925,29 @@
         <v>#NAME?</v>
       </c>
       <c r="O24" s="20"/>
-      <c r="R24" s="42" t="str">
+      <c r="R24" s="40" t="str">
         <v>C6</v>
       </c>
-      <c r="S24" s="42">
-        <v>0</v>
-      </c>
-      <c r="T24" s="42">
-        <v>0</v>
-      </c>
-      <c r="U24" s="42">
-        <v>0</v>
-      </c>
-      <c r="V24" s="42">
-        <v>0</v>
-      </c>
-      <c r="W24" s="42">
+      <c r="S24" s="40">
+        <v>0</v>
+      </c>
+      <c r="T24" s="40">
+        <v>0</v>
+      </c>
+      <c r="U24" s="40">
+        <v>0</v>
+      </c>
+      <c r="V24" s="40">
+        <v>0</v>
+      </c>
+      <c r="W24" s="40">
         <v>258</v>
       </c>
-      <c r="Y24" s="3">
-        <v>6</v>
+      <c r="Y24" s="3" t="str">
+        <v>C6</v>
       </c>
       <c r="Z24" s="3">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="AA24" s="3">
         <v>0</v>
@@ -6930,29 +6982,29 @@
         <v>#NAME?</v>
       </c>
       <c r="O25" s="20"/>
-      <c r="R25" s="42" t="str">
+      <c r="R25" s="40" t="str">
         <v>C7</v>
       </c>
-      <c r="S25" s="42">
-        <v>0</v>
-      </c>
-      <c r="T25" s="42">
-        <v>0</v>
-      </c>
-      <c r="U25" s="42">
-        <v>0</v>
-      </c>
-      <c r="V25" s="42">
-        <v>0</v>
-      </c>
-      <c r="W25" s="42">
+      <c r="S25" s="40">
+        <v>0</v>
+      </c>
+      <c r="T25" s="40">
+        <v>0</v>
+      </c>
+      <c r="U25" s="40">
+        <v>0</v>
+      </c>
+      <c r="V25" s="40">
+        <v>0</v>
+      </c>
+      <c r="W25" s="40">
         <v>369</v>
       </c>
-      <c r="Y25" s="3">
-        <v>7</v>
+      <c r="Y25" s="3" t="str">
+        <v>C7</v>
       </c>
       <c r="Z25" s="3">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="AA25" s="3">
         <v>0</v>
@@ -6987,29 +7039,29 @@
         <v>#NAME?</v>
       </c>
       <c r="O26" s="20"/>
-      <c r="R26" s="42" t="str">
+      <c r="R26" s="40" t="str">
         <v>C8</v>
       </c>
-      <c r="S26" s="42">
-        <v>0</v>
-      </c>
-      <c r="T26" s="42">
-        <v>0</v>
-      </c>
-      <c r="U26" s="42">
-        <v>0</v>
-      </c>
-      <c r="V26" s="42">
-        <v>0</v>
-      </c>
-      <c r="W26" s="42">
+      <c r="S26" s="40">
+        <v>0</v>
+      </c>
+      <c r="T26" s="40">
+        <v>0</v>
+      </c>
+      <c r="U26" s="40">
+        <v>0</v>
+      </c>
+      <c r="V26" s="40">
+        <v>0</v>
+      </c>
+      <c r="W26" s="40">
         <v>418</v>
       </c>
-      <c r="Y26" s="3">
-        <v>8</v>
+      <c r="Y26" s="3" t="str">
+        <v>C8</v>
       </c>
       <c r="Z26" s="3">
-        <v>410</v>
+        <v>418</v>
       </c>
       <c r="AA26" s="3">
         <v>0</v>
@@ -7044,29 +7096,29 @@
         <v>#NAME?</v>
       </c>
       <c r="O27" s="20"/>
-      <c r="R27" s="42" t="str">
+      <c r="R27" s="40" t="str">
         <v>C9</v>
       </c>
-      <c r="S27" s="42">
-        <v>0</v>
-      </c>
-      <c r="T27" s="42">
-        <v>0</v>
-      </c>
-      <c r="U27" s="42">
-        <v>0</v>
-      </c>
-      <c r="V27" s="42">
-        <v>0</v>
-      </c>
-      <c r="W27" s="42">
+      <c r="S27" s="40">
+        <v>0</v>
+      </c>
+      <c r="T27" s="40">
+        <v>0</v>
+      </c>
+      <c r="U27" s="40">
+        <v>0</v>
+      </c>
+      <c r="V27" s="40">
+        <v>0</v>
+      </c>
+      <c r="W27" s="40">
         <v>308</v>
       </c>
-      <c r="Y27" s="3">
-        <v>9</v>
+      <c r="Y27" s="3" t="str">
+        <v>C9</v>
       </c>
       <c r="Z27" s="3">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="AA27" s="3">
         <v>0</v>
@@ -7101,29 +7153,29 @@
         <v>#NAME?</v>
       </c>
       <c r="O28" s="20"/>
-      <c r="R28" s="42" t="str">
+      <c r="R28" s="40" t="str">
         <v>C10</v>
       </c>
-      <c r="S28" s="42">
-        <v>0</v>
-      </c>
-      <c r="T28" s="42">
-        <v>0</v>
-      </c>
-      <c r="U28" s="42">
-        <v>0</v>
-      </c>
-      <c r="V28" s="42">
-        <v>0</v>
-      </c>
-      <c r="W28" s="42">
+      <c r="S28" s="40">
+        <v>0</v>
+      </c>
+      <c r="T28" s="40">
+        <v>0</v>
+      </c>
+      <c r="U28" s="40">
+        <v>0</v>
+      </c>
+      <c r="V28" s="40">
+        <v>0</v>
+      </c>
+      <c r="W28" s="40">
         <v>410</v>
       </c>
-      <c r="Y28" s="3">
-        <v>10</v>
+      <c r="Y28" s="3" t="str">
+        <v>C10</v>
       </c>
       <c r="Z28" s="3">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="AA28" s="3">
         <v>0</v>
@@ -7158,29 +7210,29 @@
         <v>#NAME?</v>
       </c>
       <c r="O29" s="20"/>
-      <c r="R29" s="42" t="str">
+      <c r="R29" s="40" t="str">
         <v>C11</v>
       </c>
-      <c r="S29" s="42">
-        <v>0</v>
-      </c>
-      <c r="T29" s="42">
-        <v>0</v>
-      </c>
-      <c r="U29" s="42">
-        <v>0</v>
-      </c>
-      <c r="V29" s="42">
-        <v>0</v>
-      </c>
-      <c r="W29" s="42">
-        <v>0</v>
-      </c>
-      <c r="Y29" s="3">
-        <v>11</v>
+      <c r="S29" s="40">
+        <v>0</v>
+      </c>
+      <c r="T29" s="40">
+        <v>0</v>
+      </c>
+      <c r="U29" s="40">
+        <v>0</v>
+      </c>
+      <c r="V29" s="40">
+        <v>0</v>
+      </c>
+      <c r="W29" s="40">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="3" t="str">
+        <v>C11</v>
       </c>
       <c r="Z29" s="3">
-        <v>480</v>
+        <v>491</v>
       </c>
       <c r="AA29" s="3">
         <v>0</v>
@@ -7215,29 +7267,29 @@
         <v>#NAME?</v>
       </c>
       <c r="O30" s="20"/>
-      <c r="R30" s="42" t="str">
+      <c r="R30" s="40" t="str">
         <v>C12</v>
       </c>
-      <c r="S30" s="42">
-        <v>0</v>
-      </c>
-      <c r="T30" s="42">
-        <v>0</v>
-      </c>
-      <c r="U30" s="42">
-        <v>0</v>
-      </c>
-      <c r="V30" s="42">
-        <v>0</v>
-      </c>
-      <c r="W30" s="42">
-        <v>0</v>
-      </c>
-      <c r="Y30" s="3">
-        <v>12</v>
+      <c r="S30" s="40">
+        <v>0</v>
+      </c>
+      <c r="T30" s="40">
+        <v>0</v>
+      </c>
+      <c r="U30" s="40">
+        <v>0</v>
+      </c>
+      <c r="V30" s="40">
+        <v>0</v>
+      </c>
+      <c r="W30" s="40">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="3" t="str">
+        <v>C12</v>
       </c>
       <c r="Z30" s="3">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="AA30" s="3">
         <v>0</v>
@@ -7665,9 +7717,6 @@
     <row r="72" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O72" s="20"/>
     </row>
-    <row r="73" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O73" s="20"/>
-    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
@@ -7676,6 +7725,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Reviewing the Youtube video of the solution
</commit_message>
<xml_diff>
--- a/CH-060 Match payments.xlsx
+++ b/CH-060 Match payments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6668F7-480C-4C64-922B-8D250C0BEB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C678E37-EB6F-4670-9FDB-D6D64E325D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="Alternate" sheetId="3" r:id="rId3"/>
     <sheet name="Alternate2" sheetId="4" r:id="rId4"/>
     <sheet name="Alternate3" sheetId="5" r:id="rId5"/>
+    <sheet name="Scratch" sheetId="6" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Alternate!$B$2:$B$15</definedName>
@@ -28,6 +29,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Alternate3!$B$2:$B$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$B$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$B$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Scratch!$B$2:$B$15</definedName>
     <definedName name="_na">Alternate3!$E$48:$E$51</definedName>
     <definedName name="allocate_payment">_xlfn.LAMBDA(_xlpm.costs,_xlpm.payments,_xlpm.allocations,_xlpm.position, _xlfn.LET(_xlpm._costRows, ROWS(_xlpm.costs), _xlpm._paymentColumns, COLUMNS(_xlpm.payments), _xlpm._seq, _xlfn.WRAPCOLS(_xlfn.SEQUENCE(_xlpm._costRows * _xlpm._paymentColumns), _xlpm._costRows), _xlpm._col, INT((_xlpm.position - 1) / _xlpm._costRows) + 1, _xlpm._row, MOD(_xlpm.position - 1, _xlpm._costRows) + 1, _xlpm._cost, INDEX(_xlpm.costs, _xlpm._row, 1), _xlpm._payment, INDEX(_xlpm.payments, 1, _xlpm._col), _xlpm._newAllocation, IF(_xlpm._cost &lt;= _xlpm._payment, _xlpm._cost, _xlpm._payment), _xlpm._newAllocations, IF(_xlpm._seq = _xlpm.position, _xlpm._newAllocation, 0) + _xlpm.allocations, _xlpm._newTotal, _xlfn.LAMBDA(_xlpm.seq,_xlpm.pos,_xlpm.arr, IF(_xlpm.seq = _xlpm.pos, _xlpm.arr - _xlpm._newAllocation, _xlpm.arr)), _xlpm._newCosts, _xlpm._newTotal(_xlfn.SEQUENCE(_xlpm._costRows), _xlpm._row, _xlpm.costs), _xlpm._newPayments, _xlpm._newTotal(_xlfn.SEQUENCE(, _xlpm._paymentColumns), _xlpm._col, _xlpm.payments), IF((_xlpm.position + 1) &gt; MAX(_xlpm._seq), _xlpm._newAllocations, allocate_payment(_xlpm._newCosts, _xlpm._newPayments, _xlpm._newAllocations, _xlpm.position + 1))))</definedName>
     <definedName name="allocate_payments_usage">_xlfn.LET(_xlpm.costs, [1]Sheet1!B1048560:B1048571, _xlpm.payments, _xlfn.TOROW([1]Sheet1!F1048560:F1048564), _xlpm.empty_array, _xlfn.MAKEARRAY(ROWS(_xlpm.costs), COLUMNS(_xlpm.payments), _xlfn.LAMBDA(_xlpm.r,_xlpm.c, 0)), _xlpm.header, _xlfn.HSTACK("", _xlfn.TOROW([1]Sheet1!D1048560:D1048564)), _xlfn.VSTACK(_xlpm.header, _xlfn.HSTACK([1]Sheet1!XFD1048560:XFD1048571, allocate_payment(_xlpm.costs, _xlpm.payments, _xlpm.empty_array, 1))))</definedName>
@@ -35,6 +37,7 @@
     <definedName name="Trial.allocate_payments_usage">_xlfn.LET(_xlpm.costs, [1]Sheet1!B1048560:B1048571, _xlpm.payments, _xlfn.TOROW([1]Sheet1!F1048560:F1048564), _xlpm.empty_array, _xlfn.MAKEARRAY(ROWS(_xlpm.costs), COLUMNS(_xlpm.payments), _xlfn.LAMBDA(_xlpm.r,_xlpm.c, 0)), _xlpm.header, _xlfn.HSTACK("", _xlfn.TOROW([1]Sheet1!D1048560:D1048564)), _xlfn.VSTACK(_xlpm.header, _xlfn.HSTACK([1]Sheet1!XFD1048560:XFD1048571, Trial.allocate_payment(_xlpm.costs, _xlpm.payments, _xlpm.empty_array, 1))))</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -77,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="28">
   <si>
     <t>Result</t>
   </si>
@@ -158,6 +161,9 @@
   </si>
   <si>
     <t>I found the issue. Some problem with my Excel version.</t>
+  </si>
+  <si>
+    <t>Youtube Solution Link</t>
   </si>
 </sst>
 </file>
@@ -439,7 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -550,6 +556,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5854,8 +5863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D8F953-0749-4436-8A06-19D4F87E6D90}">
   <dimension ref="A1:AJ72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W51" sqref="W51"/>
+    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -7729,6 +7738,867 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9A81A7-D6B7-40E5-911B-C548F7BC223F}">
+  <dimension ref="B1:X74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" style="3" customWidth="1"/>
+    <col min="2" max="2" width="4.09765625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="12.19921875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="6.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.59765625" style="3"/>
+    <col min="6" max="6" width="4.19921875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.8984375" style="3" customWidth="1"/>
+    <col min="9" max="10" width="8.59765625" style="3"/>
+    <col min="11" max="16" width="6" style="3" customWidth="1"/>
+    <col min="17" max="19" width="8.59765625" style="3"/>
+    <col min="20" max="20" width="8.796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.59765625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:24" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="F1" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="K1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="R1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="7"/>
+      <c r="L2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" s="43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="10">
+        <v>45325</v>
+      </c>
+      <c r="D3" s="29">
+        <v>120</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="12">
+        <v>45278</v>
+      </c>
+      <c r="H3" s="31">
+        <v>600</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="33">
+        <v>120</v>
+      </c>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="15"/>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="16">
+        <v>45338</v>
+      </c>
+      <c r="D4" s="30">
+        <v>356</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="12">
+        <v>45286</v>
+      </c>
+      <c r="H4" s="31">
+        <v>50</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="33">
+        <v>356</v>
+      </c>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="34"/>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="16">
+        <v>45341</v>
+      </c>
+      <c r="D5" s="30">
+        <v>312</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="12">
+        <v>45312</v>
+      </c>
+      <c r="H5" s="31">
+        <v>112</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="33">
+        <v>124</v>
+      </c>
+      <c r="M5" s="33">
+        <v>50</v>
+      </c>
+      <c r="N5" s="33">
+        <v>112</v>
+      </c>
+      <c r="O5" s="33">
+        <v>26</v>
+      </c>
+      <c r="P5" s="34"/>
+      <c r="T5" s="3">
+        <v>600</v>
+      </c>
+      <c r="U5" s="3">
+        <v>50</v>
+      </c>
+      <c r="V5" s="3">
+        <v>112</v>
+      </c>
+      <c r="W5" s="3">
+        <v>800</v>
+      </c>
+      <c r="X5" s="3">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="16">
+        <v>45355</v>
+      </c>
+      <c r="D6" s="30">
+        <v>437</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="12">
+        <v>45315</v>
+      </c>
+      <c r="H6" s="31">
+        <v>800</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33">
+        <v>437</v>
+      </c>
+      <c r="P6" s="34"/>
+      <c r="R6" s="29">
+        <v>120</v>
+      </c>
+      <c r="T6" s="3" cm="1">
+        <f t="array" ref="T6:T17">_xlfn.DROP(_xlfn.REDUCE(T5,$R$6:$R$17-_xlfn.BYROW($S$6:S17,_xlfn.LAMBDA(_xlpm.r,SUM(_xlpm.r))),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,MIN(_xlpm.v,_xlfn.SINGLE(_xlpm.a)*2-SUM(_xlpm.a))))),1)</f>
+        <v>120</v>
+      </c>
+      <c r="U6" s="3" cm="1">
+        <f t="array" ref="U6:U17">_xlfn.DROP(_xlfn.REDUCE(U5,$R$6:$R$17-_xlfn.BYROW($S$6:T17,_xlfn.LAMBDA(_xlpm.r,SUM(_xlpm.r))),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,MIN(_xlpm.v,_xlfn.SINGLE(_xlpm.a)*2-SUM(_xlpm.a))))),1)</f>
+        <v>0</v>
+      </c>
+      <c r="V6" s="3" cm="1">
+        <f t="array" ref="V6:V17">_xlfn.DROP(_xlfn.REDUCE(V5,$R$6:$R$17-_xlfn.BYROW($S$6:U17,_xlfn.LAMBDA(_xlpm.r,SUM(_xlpm.r))),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,MIN(_xlpm.v,_xlfn.SINGLE(_xlpm.a)*2-SUM(_xlpm.a))))),1)</f>
+        <v>0</v>
+      </c>
+      <c r="W6" s="3" cm="1">
+        <f t="array" ref="W6:W17">_xlfn.DROP(_xlfn.REDUCE(W5,$R$6:$R$17-_xlfn.BYROW($S$6:V17,_xlfn.LAMBDA(_xlpm.r,SUM(_xlpm.r))),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,MIN(_xlpm.v,_xlfn.SINGLE(_xlpm.a)*2-SUM(_xlpm.a))))),1)</f>
+        <v>0</v>
+      </c>
+      <c r="X6" s="3" cm="1">
+        <f t="array" ref="X6:X17">_xlfn.DROP(_xlfn.REDUCE(X5,$R$6:$R$17-_xlfn.BYROW($S$6:W17,_xlfn.LAMBDA(_xlpm.r,SUM(_xlpm.r))),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,MIN(_xlpm.v,_xlfn.SINGLE(_xlpm.a)*2-SUM(_xlpm.a))))),1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="16">
+        <v>45364</v>
+      </c>
+      <c r="D7" s="30">
+        <v>374</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="19">
+        <v>45327</v>
+      </c>
+      <c r="H7" s="32">
+        <v>1800</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33">
+        <v>337</v>
+      </c>
+      <c r="P7" s="34">
+        <v>37</v>
+      </c>
+      <c r="R7" s="30">
+        <v>356</v>
+      </c>
+      <c r="T7" s="3">
+        <v>356</v>
+      </c>
+      <c r="U7" s="3">
+        <v>0</v>
+      </c>
+      <c r="V7" s="3">
+        <v>0</v>
+      </c>
+      <c r="W7" s="3">
+        <v>0</v>
+      </c>
+      <c r="X7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="16">
+        <v>45365</v>
+      </c>
+      <c r="D8" s="30">
+        <v>258</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="34">
+        <v>258</v>
+      </c>
+      <c r="R8" s="30">
+        <v>312</v>
+      </c>
+      <c r="T8" s="3">
+        <v>124</v>
+      </c>
+      <c r="U8" s="3">
+        <v>50</v>
+      </c>
+      <c r="V8" s="3">
+        <v>112</v>
+      </c>
+      <c r="W8" s="3">
+        <v>26</v>
+      </c>
+      <c r="X8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="16">
+        <v>45370</v>
+      </c>
+      <c r="D9" s="30">
+        <v>369</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="17"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="34">
+        <v>369</v>
+      </c>
+      <c r="R9" s="30">
+        <v>437</v>
+      </c>
+      <c r="T9" s="3">
+        <v>0</v>
+      </c>
+      <c r="U9" s="3">
+        <v>0</v>
+      </c>
+      <c r="V9" s="3">
+        <v>0</v>
+      </c>
+      <c r="W9" s="3">
+        <v>437</v>
+      </c>
+      <c r="X9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="16">
+        <v>45376</v>
+      </c>
+      <c r="D10" s="30">
+        <v>418</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="17"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="34">
+        <v>418</v>
+      </c>
+      <c r="R10" s="30">
+        <v>374</v>
+      </c>
+      <c r="T10" s="3">
+        <v>0</v>
+      </c>
+      <c r="U10" s="3">
+        <v>0</v>
+      </c>
+      <c r="V10" s="3">
+        <v>0</v>
+      </c>
+      <c r="W10" s="3">
+        <v>337</v>
+      </c>
+      <c r="X10" s="3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="16">
+        <v>45384</v>
+      </c>
+      <c r="D11" s="30">
+        <v>308</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="17"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="34">
+        <v>308</v>
+      </c>
+      <c r="R11" s="30">
+        <v>258</v>
+      </c>
+      <c r="T11" s="3">
+        <v>0</v>
+      </c>
+      <c r="U11" s="3">
+        <v>0</v>
+      </c>
+      <c r="V11" s="3">
+        <v>0</v>
+      </c>
+      <c r="W11" s="3">
+        <v>0</v>
+      </c>
+      <c r="X11" s="3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="16">
+        <v>45397</v>
+      </c>
+      <c r="D12" s="30">
+        <v>410</v>
+      </c>
+      <c r="G12" s="20"/>
+      <c r="K12" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="17"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="34">
+        <v>410</v>
+      </c>
+      <c r="R12" s="30">
+        <v>369</v>
+      </c>
+      <c r="T12" s="3">
+        <v>0</v>
+      </c>
+      <c r="U12" s="3">
+        <v>0</v>
+      </c>
+      <c r="V12" s="3">
+        <v>0</v>
+      </c>
+      <c r="W12" s="3">
+        <v>0</v>
+      </c>
+      <c r="X12" s="3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="16">
+        <v>45406</v>
+      </c>
+      <c r="D13" s="30">
+        <v>491</v>
+      </c>
+      <c r="G13" s="20"/>
+      <c r="K13" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="P13" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="R13" s="30">
+        <v>418</v>
+      </c>
+      <c r="T13" s="3">
+        <v>0</v>
+      </c>
+      <c r="U13" s="3">
+        <v>0</v>
+      </c>
+      <c r="V13" s="3">
+        <v>0</v>
+      </c>
+      <c r="W13" s="3">
+        <v>0</v>
+      </c>
+      <c r="X13" s="3">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="16">
+        <v>45409</v>
+      </c>
+      <c r="D14" s="30">
+        <v>50</v>
+      </c>
+      <c r="G14" s="20"/>
+      <c r="K14" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="O14" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="P14" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="R14" s="30">
+        <v>308</v>
+      </c>
+      <c r="T14" s="3">
+        <v>0</v>
+      </c>
+      <c r="U14" s="3">
+        <v>0</v>
+      </c>
+      <c r="V14" s="3">
+        <v>0</v>
+      </c>
+      <c r="W14" s="3">
+        <v>0</v>
+      </c>
+      <c r="X14" s="3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="G15" s="20"/>
+      <c r="L15" s="27"/>
+      <c r="O15" s="20"/>
+      <c r="R15" s="30">
+        <v>410</v>
+      </c>
+      <c r="T15" s="3">
+        <v>0</v>
+      </c>
+      <c r="U15" s="3">
+        <v>0</v>
+      </c>
+      <c r="V15" s="3">
+        <v>0</v>
+      </c>
+      <c r="W15" s="3">
+        <v>0</v>
+      </c>
+      <c r="X15" s="3">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="G16" s="20"/>
+      <c r="L16" s="27"/>
+      <c r="O16" s="20"/>
+      <c r="R16" s="30">
+        <v>491</v>
+      </c>
+      <c r="T16" s="3">
+        <v>0</v>
+      </c>
+      <c r="U16" s="3">
+        <v>0</v>
+      </c>
+      <c r="V16" s="3">
+        <v>0</v>
+      </c>
+      <c r="W16" s="3">
+        <v>0</v>
+      </c>
+      <c r="X16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="G17" s="20"/>
+      <c r="L17" s="27"/>
+      <c r="O17" s="20"/>
+      <c r="R17" s="30">
+        <v>50</v>
+      </c>
+      <c r="T17" s="3">
+        <v>0</v>
+      </c>
+      <c r="U17" s="3">
+        <v>0</v>
+      </c>
+      <c r="V17" s="3">
+        <v>0</v>
+      </c>
+      <c r="W17" s="3">
+        <v>0</v>
+      </c>
+      <c r="X17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="G18" s="20"/>
+      <c r="L18" s="27"/>
+      <c r="O18" s="20"/>
+    </row>
+    <row r="19" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="L19" s="20"/>
+      <c r="O19" s="20"/>
+    </row>
+    <row r="20" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="L20" s="20"/>
+      <c r="O20" s="20"/>
+    </row>
+    <row r="21" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="L21" s="20"/>
+      <c r="O21" s="20"/>
+    </row>
+    <row r="22" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="L22" s="20"/>
+      <c r="O22" s="20"/>
+    </row>
+    <row r="23" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="L23" s="20"/>
+      <c r="O23" s="20"/>
+    </row>
+    <row r="24" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="L24" s="20"/>
+      <c r="O24" s="20"/>
+    </row>
+    <row r="25" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="L25" s="20"/>
+      <c r="O25" s="20"/>
+    </row>
+    <row r="26" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="L26" s="20"/>
+      <c r="O26" s="20"/>
+    </row>
+    <row r="27" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="L27" s="20"/>
+      <c r="O27" s="20"/>
+    </row>
+    <row r="28" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="L28" s="20"/>
+      <c r="O28" s="20"/>
+    </row>
+    <row r="29" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="O29" s="20"/>
+    </row>
+    <row r="30" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="O30" s="20"/>
+    </row>
+    <row r="31" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="O31" s="20"/>
+    </row>
+    <row r="32" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="O32" s="20"/>
+    </row>
+    <row r="33" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O33" s="20"/>
+    </row>
+    <row r="34" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O34" s="20"/>
+    </row>
+    <row r="35" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O35" s="20"/>
+    </row>
+    <row r="36" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O36" s="20"/>
+    </row>
+    <row r="37" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O37" s="20"/>
+    </row>
+    <row r="38" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O38" s="20"/>
+    </row>
+    <row r="39" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O39" s="20"/>
+    </row>
+    <row r="40" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O40" s="20"/>
+    </row>
+    <row r="41" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O41" s="20"/>
+    </row>
+    <row r="42" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O42" s="20"/>
+    </row>
+    <row r="43" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O43" s="20"/>
+    </row>
+    <row r="44" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O44" s="20"/>
+    </row>
+    <row r="45" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O45" s="20"/>
+    </row>
+    <row r="46" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O46" s="20"/>
+    </row>
+    <row r="47" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O47" s="20"/>
+    </row>
+    <row r="48" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O48" s="20"/>
+    </row>
+    <row r="49" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O49" s="20"/>
+    </row>
+    <row r="50" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O50" s="20"/>
+    </row>
+    <row r="51" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O51" s="20"/>
+    </row>
+    <row r="52" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O52" s="20"/>
+    </row>
+    <row r="53" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O53" s="20"/>
+    </row>
+    <row r="54" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O54" s="20"/>
+    </row>
+    <row r="55" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O55" s="20"/>
+    </row>
+    <row r="56" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O56" s="20"/>
+    </row>
+    <row r="57" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O57" s="20"/>
+    </row>
+    <row r="58" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O58" s="20"/>
+    </row>
+    <row r="59" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O59" s="20"/>
+    </row>
+    <row r="60" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O60" s="20"/>
+    </row>
+    <row r="61" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O61" s="20"/>
+    </row>
+    <row r="62" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O62" s="20"/>
+    </row>
+    <row r="63" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O63" s="20"/>
+    </row>
+    <row r="64" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O64" s="20"/>
+    </row>
+    <row r="65" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O65" s="20"/>
+    </row>
+    <row r="66" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O66" s="20"/>
+    </row>
+    <row r="67" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O67" s="20"/>
+    </row>
+    <row r="68" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O68" s="20"/>
+    </row>
+    <row r="69" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O69" s="20"/>
+    </row>
+    <row r="70" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O70" s="20"/>
+    </row>
+    <row r="71" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O71" s="20"/>
+    </row>
+    <row r="72" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O72" s="20"/>
+    </row>
+    <row r="73" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O73" s="20"/>
+    </row>
+    <row r="74" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O74" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="K1:P1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="R2" r:id="rId1" xr:uid="{3EB1206F-E544-45FC-B2C2-9A2BF5481D91}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AYQBsAGwAbwBjAGEAdABlAF8AcABhAHkAbQBlAG4AdAAgAD0AIABMAEEATQBCAEQAQQAoAGMAbwBzAHQAcwAsACAAcABhAHkAbQBlAG4AdABzACwAIABhAGwAbABvAGMAYQB0AGkAbwBuAHMALAAgAHAAbwBzAGkAdABpAG8AbgAsACAAXABuAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABfAGMAbwBzAHQAUgBvAHcAcwAsAFIATwBXAFMAKABjAG8AcwB0AHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXwBwAGEAeQBtAGUAbgB0AEMAbwBsAHUAbQBuAHMALABDAE8ATABVAE0ATgBTACgAcABhAHkAbQBlAG4AdABzACkALABcAG4AIAAgACAAIAAgACAAIAAgAF8AcwBlAHEALAAgAFcAUgBBAFAAQwBPAEwAUwAoAFMARQBRAFUARQBOAEMARQAoAF8AYwBvAHMAdABSAG8AdwBzACoAXwBwAGEAeQBtAGUAbgB0AEMAbwBsAHUAbQBuAHMAKQAsAF8AYwBvAHMAdABSAG8AdwBzACkALABcAG4AIAAgACAAIAAgACAAIAAgAF8AYwBvAGwALAAgAEkATgBUACgAKABwAG8AcwBpAHQAaQBvAG4AIAAtACAAMQApACAALwAgAF8AYwBvAHMAdABSAG8AdwBzACkAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAXwByAG8AdwAsACAATQBPAEQAKABwAG8AcwBpAHQAaQBvAG4AIAAtACAAMQAsACAAXwBjAG8AcwB0AFIAbwB3AHMAKQAgACsAIAAxACwAXABuACAAIAAgACAAIAAgACAAIABfAGMAbwBzAHQALAAgAEkATgBEAEUAWAAoAGMAbwBzAHQAcwAsAF8AcgBvAHcALAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgAF8AcABhAHkAbQBlAG4AdAAsACAASQBOAEQARQBYACgAcABhAHkAbQBlAG4AdABzACwAMQAsAF8AYwBvAGwAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXwBuAGUAdwBBAGwAbABvAGMAYQB0AGkAbwBuACwAIABJAEYAKABfAGMAbwBzAHQAPAA9AF8AcABhAHkAbQBlAG4AdAAsAF8AYwBvAHMAdAAsAF8AcABhAHkAbQBlAG4AdAApACwAXABuACAAIAAgACAAIAAgACAAIABfAG4AZQB3AEEAbABsAG8AYwBhAHQAaQBvAG4AcwAsACAASQBGACgAXwBzAGUAcQA9AHAAbwBzAGkAdABpAG8AbgAsAF8AbgBlAHcAQQBsAGwAbwBjAGEAdABpAG8AbgAsADAAKQArAGEAbABsAG8AYwBhAHQAaQBvAG4AcwAsAFwAbgAgACAAIAAgACAAIAAgACAAXwBuAGUAdwBUAG8AdABhAGwALABMAEEATQBCAEQAQQAoAHMAZQBxACwAcABvAHMALABhAHIAcgAsAEkARgAoAHMAZQBxAD0AcABvAHMALABhAHIAcgAtAF8AbgBlAHcAQQBsAGwAbwBjAGEAdABpAG8AbgAsAGEAcgByACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXwBuAGUAdwBDAG8AcwB0AHMALABfAG4AZQB3AFQAbwB0AGEAbAAoAFMARQBRAFUARQBOAEMARQAoAF8AYwBvAHMAdABSAG8AdwBzACkALABfAHIAbwB3ACwAYwBvAHMAdABzACkALABcAG4AIAAgACAAIAAgACAAIAAgAF8AbgBlAHcAUABhAHkAbQBlAG4AdABzACwAXwBuAGUAdwBUAG8AdABhAGwAKABTAEUAUQBVAEUATgBDAEUAKAAsAF8AcABhAHkAbQBlAG4AdABDAG8AbAB1AG0AbgBzACkALABfAGMAbwBsACwAcABhAHkAbQBlAG4AdABzACkALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAoAHAAbwBzAGkAdABpAG8AbgAgACsAIAAxACkAPgAgAE0AQQBYACgAXwBzAGUAcQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAF8AbgBlAHcAQQBsAGwAbwBjAGEAdABpAG8AbgBzACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGEAbABsAG8AYwBhAHQAZQBfAHAAYQB5AG0AZQBuAHQAKABfAG4AZQB3AEMAbwBzAHQAcwAsAF8AbgBlAHcAUABhAHkAbQBlAG4AdABzACwAXwBuAGUAdwBBAGwAbABvAGMAYQB0AGkAbwBuAHMALABwAG8AcwBpAHQAaQBvAG4AIAArACAAMQApACAAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAGEAbABsAG8AYwBhAHQAZQBfAHAAYQB5AG0AZQBuAHQAcwBfAHUAcwBhAGcAZQAgAD0AXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAGMAbwBzAHQAcwAsAFMAaABlAGUAdAAxACEARAA0ADoARAAxADUALABcAG4AIAAgACAAIAAgACAAIAAgAHAAYQB5AG0AZQBuAHQAcwAsAFQATwBSAE8AVwAoAFMAaABlAGUAdAAxACEASAA0ADoASAA4ACkALABcAG4AIAAgACAAIAAgACAAIAAgAGUAbQBwAHQAeQBfAGEAcgByAGEAeQAsAE0AQQBLAEUAQQBSAFIAQQBZACgAUgBPAFcAUwAoAGMAbwBzAHQAcwApACwAQwBPAEwAVQBNAE4AUwAoAHAAYQB5AG0AZQBuAHQAcwApACwATABBAE0AQgBEAEEAKAByACwAYwAsADAAKQApACwAXABuACAAIAAgACAAIAAgACAAIABoAGUAYQBkAGUAcgAsAEgAUwBUAEEAQwBLACgAXAAiAFwAIgAsAFQATwBSAE8AVwAoAFMAaABlAGUAdAAxACEARgA0ADoARgA4ACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAVgBTAFQAQQBDAEsAKABoAGUAYQBkAGUAcgAsAEgAUwBUAEEAQwBLACgAUwBoAGUAZQB0ADEAIQBCADQAOgBCADEANQAsAGEAbABsAG8AYwBhAHQAZQBfAHAAYQB5AG0AZQBuAHQAKABjAG8AcwB0AHMALABwAGEAeQBtAGUAbgB0AHMALABlAG0AcAB0AHkAXwBhAHIAcgBhAHkALAAxACkAKQApAFwAbgAgACAAIAAgACkAOwAiAH0ALAB7ACIAcABhAHQAaAAiADoAIgAvAHAAcgBvAGoAZQBjAHQAcwAvAFQAcgBpAGEAbAAiACwAIgB0AGUAeAB0ACIAOgAiAGEAbABsAG8AYwBhAHQAZQBfAHAAYQB5AG0AZQBuAHQAIAA9ACAATABBAE0AQgBEAEEAKABjAG8AcwB0AHMALAAgAHAAYQB5AG0AZQBuAHQAcwAsACAAYQBsAGwAbwBjAGEAdABpAG8AbgBzACwAIABwAG8AcwBpAHQAaQBvAG4ALAAgAFwAbgBcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAXwBjAG8AcwB0AFIAbwB3AHMALABSAE8AVwBTACgAYwBvAHMAdABzACkALABcAG4AIAAgACAAIAAgACAAIAAgAF8AcABhAHkAbQBlAG4AdABDAG8AbAB1AG0AbgBzACwAQwBPAEwAVQBNAE4AUwAoAHAAYQB5AG0AZQBuAHQAcwApACwAXABuACAAIAAgACAAIAAgACAAIABfAHMAZQBxACwAIABXAFIAQQBQAEMATwBMAFMAKABTAEUAUQBVAEUATgBDAEUAKABfAGMAbwBzAHQAUgBvAHcAcwAqAF8AcABhAHkAbQBlAG4AdABDAG8AbAB1AG0AbgBzACkALABfAGMAbwBzAHQAUgBvAHcAcwApACwAXABuACAAIAAgACAAIAAgACAAIABfAGMAbwBsACwAIABJAE4AVAAoACgAcABvAHMAaQB0AGkAbwBuACAALQAgADEAKQAgAC8AIABfAGMAbwBzAHQAUgBvAHcAcwApACAAKwAgADEALABcAG4AIAAgACAAIAAgACAAIAAgAF8AcgBvAHcALAAgAE0ATwBEACgAcABvAHMAaQB0AGkAbwBuACAALQAgADEALAAgAF8AYwBvAHMAdABSAG8AdwBzACkAIAArACAAMQAsAFwAbgAgACAAIAAgACAAIAAgACAAXwBjAG8AcwB0ACwAIABJAE4ARABFAFgAKABjAG8AcwB0AHMALABfAHIAbwB3ACwAMQApACwAXABuACAAIAAgACAAIAAgACAAIABfAHAAYQB5AG0AZQBuAHQALAAgAEkATgBEAEUAWAAoAHAAYQB5AG0AZQBuAHQAcwAsADEALABfAGMAbwBsACkALABcAG4AIAAgACAAIAAgACAAIAAgAF8AbgBlAHcAQQBsAGwAbwBjAGEAdABpAG8AbgAsACAASQBGACgAXwBjAG8AcwB0ADwAPQBfAHAAYQB5AG0AZQBuAHQALABfAGMAbwBzAHQALABfAHAAYQB5AG0AZQBuAHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXwBuAGUAdwBBAGwAbABvAGMAYQB0AGkAbwBuAHMALAAgAEkARgAoAF8AcwBlAHEAPQBwAG8AcwBpAHQAaQBvAG4ALABfAG4AZQB3AEEAbABsAG8AYwBhAHQAaQBvAG4ALAAwACkAKwBhAGwAbABvAGMAYQB0AGkAbwBuAHMALABcAG4AIAAgACAAIAAgACAAIAAgAF8AbgBlAHcAVABvAHQAYQBsACwATABBAE0AQgBEAEEAKABzAGUAcQAsAHAAbwBzACwAYQByAHIALABJAEYAKABzAGUAcQA9AHAAbwBzACwAYQByAHIALQBfAG4AZQB3AEEAbABsAG8AYwBhAHQAaQBvAG4ALABhAHIAcgApACkALABcAG4AIAAgACAAIAAgACAAIAAgAF8AbgBlAHcAQwBvAHMAdABzACwAXwBuAGUAdwBUAG8AdABhAGwAKABTAEUAUQBVAEUATgBDAEUAKABfAGMAbwBzAHQAUgBvAHcAcwApACwAXwByAG8AdwAsAGMAbwBzAHQAcwApACwAXABuACAAIAAgACAAIAAgACAAIABfAG4AZQB3AFAAYQB5AG0AZQBuAHQAcwAsAF8AbgBlAHcAVABvAHQAYQBsACgAUwBFAFEAVQBFAE4AQwBFACgALABfAHAAYQB5AG0AZQBuAHQAQwBvAGwAdQBtAG4AcwApACwAXwBjAG8AbAAsAHAAYQB5AG0AZQBuAHQAcwApACwAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAKABwAG8AcwBpAHQAaQBvAG4AIAArACAAMQApAD4AIABNAEEAWAAoAF8AcwBlAHEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABfAG4AZQB3AEEAbABsAG8AYwBhAHQAaQBvAG4AcwAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABhAGwAbABvAGMAYQB0AGUAXwBwAGEAeQBtAGUAbgB0ACgAXwBuAGUAdwBDAG8AcwB0AHMALABfAG4AZQB3AFAAYQB5AG0AZQBuAHQAcwAsAF8AbgBlAHcAQQBsAGwAbwBjAGEAdABpAG8AbgBzACwAcABvAHMAaQB0AGkAbwBuACAAKwAgADEAKQAgAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBhAGwAbABvAGMAYQB0AGUAXwBwAGEAeQBtAGUAbgB0AHMAXwB1AHMAYQBnAGUAIAA9AFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABjAG8AcwB0AHMALABTAGgAZQBlAHQAMQAhAEQANAA6AEQAMQA1ACwAXABuACAAIAAgACAAIAAgACAAIABwAGEAeQBtAGUAbgB0AHMALABUAE8AUgBPAFcAKABTAGgAZQBlAHQAMQAhAEgANAA6AEgAOAApACwAXABuACAAIAAgACAAIAAgACAAIABlAG0AcAB0AHkAXwBhAHIAcgBhAHkALABNAEEASwBFAEEAUgBSAEEAWQAoAFIATwBXAFMAKABjAG8AcwB0AHMAKQAsAEMATwBMAFUATQBOAFMAKABwAGEAeQBtAGUAbgB0AHMAKQAsAEwAQQBNAEIARABBACgAcgAsAGMALAAwACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAaABlAGEAZABlAHIALABIAFMAVABBAEMASwAoAFwAIgBcACIALABUAE8AUgBPAFcAKABTAGgAZQBlAHQAMQAhAEYANAA6AEYAOAApACkALABcAG4AIAAgACAAIAAgACAAIAAgAFYAUwBUAEEAQwBLACgAaABlAGEAZABlAHIALABIAFMAVABBAEMASwAoAFMAaABlAGUAdAAxACEAQgA0ADoAQgAxADUALABhAGwAbABvAGMAYQB0AGUAXwBwAGEAeQBtAGUAbgB0ACgAYwBvAHMAdABzACwAcABhAHkAbQBlAG4AdABzACwAZQBtAHAAdAB5AF8AYQByAHIAYQB5ACwAMQApACkAKQBcAG4AIAAgACAAIAApADsAIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbACIAYQBsAGwAbwBjAGEAdABlAF8AcABhAHkAbQBlAG4AdAAiACwAIgBhAGwAbABvAGMAYQB0AGUAXwBwAGEAeQBtAGUAbgB0AHMAXwB1AHMAYQBnAGUAIgAsACIAVAByAGkAYQBsAC4AYQBsAGwAbwBjAGEAdABlAF8AcABhAHkAbQBlAG4AdAAiACwAIgBUAHIAaQBhAGwALgBhAGwAbABvAGMAYQB0AGUAXwBwAGEAeQBtAGUAbgB0AHMAXwB1AHMAYQBnAGUAIgBdACwAIgBsAG8AYwBhAGwAZQAiADoAewAiAGwAaQBzAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgByAG8AdwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgA7ACIALAAiAGMAbwBsAHUAbQBuAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAdABoAG8AdQBzAGEAbgBkAHMAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBQAG8AcwBpAHQAaQBvAG4AcwAiADoAWwAzAF0ALAAiAGQAZQBjAGkAbQBhAGwAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALgAiACwAIgBkAGEAdABlAE8AcgBkAGUAcgAiADoAIgBNAEQAWQAiACwAIgBjAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwAIgA6ACIAJAAiACwAIgBpAHMAQwB1AHIAcgBlAG4AYwB5AFMAeQBtAGIAbwBsAEwAZQBhAGQAIgA6AHQAcgB1AGUALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwBlAHAAQgB5AFMAcABhAGMAZQAiADoAZgBhAGwAcwBlACwAIgByAG8AdwBMAGUAdAB0AGUAcgAiADoAIgBSACIALAAiAGMAbwBsAHUAbQBuAEwAZQB0AHQAZQByACIAOgAiAEMAIgAsACIAcgBjAEwAZQBmAHQAQgByAGEAYwBrAGUAdAAiADoAIgBbACIALAAiAHIAYwBSAGkAZwBoAHQAQgByAGEAYwBrAGUAdAAiADoAIgBdACIALAAiAHMAdABhAHQAZQBtAGUAbgB0AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAbABvAGMAYQBsAGUATgBhAG0AZQAiADoAIgBlAG4ALQB1AHMAIgB9AH0A</AFEJSONBlob>
 </file>

</xml_diff>

<commit_message>
still trying to come up with my solution
</commit_message>
<xml_diff>
--- a/CH-060 Match payments.xlsx
+++ b/CH-060 Match payments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C678E37-EB6F-4670-9FDB-D6D64E325D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA40E6A-9F49-4489-8D60-5EE8E37A21D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,6 @@
     <definedName name="Trial.allocate_payments_usage">_xlfn.LET(_xlpm.costs, [1]Sheet1!B1048560:B1048571, _xlpm.payments, _xlfn.TOROW([1]Sheet1!F1048560:F1048564), _xlpm.empty_array, _xlfn.MAKEARRAY(ROWS(_xlpm.costs), COLUMNS(_xlpm.payments), _xlfn.LAMBDA(_xlpm.r,_xlpm.c, 0)), _xlpm.header, _xlfn.HSTACK("", _xlfn.TOROW([1]Sheet1!D1048560:D1048564)), _xlfn.VSTACK(_xlpm.header, _xlfn.HSTACK([1]Sheet1!XFD1048560:XFD1048571, Trial.allocate_payment(_xlpm.costs, _xlpm.payments, _xlpm.empty_array, 1))))</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -551,14 +550,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1934,24 +1933,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="F1" s="41" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="F1" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="K1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="K1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
       <c r="R1" s="1" t="s">
         <v>25</v>
       </c>
@@ -2556,24 +2555,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:31" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="F1" s="41" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="F1" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="K1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="K1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
       <c r="AA1" s="1" t="s">
         <v>16</v>
       </c>
@@ -4156,24 +4155,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="F1" s="41" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="F1" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="K1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="K1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
       <c r="R1" s="37" t="s">
         <v>25</v>
       </c>
@@ -5266,24 +5265,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="F1" s="41" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="F1" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="K1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="K1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -5863,8 +5862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D8F953-0749-4436-8A06-19D4F87E6D90}">
   <dimension ref="A1:AJ72"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5884,30 +5883,30 @@
     <col min="13" max="16" width="6" style="3" customWidth="1"/>
     <col min="17" max="21" width="8.59765625" style="3"/>
     <col min="22" max="22" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="8.59765625" style="3"/>
-    <col min="26" max="26" width="8.796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="8.59765625" style="3"/>
+    <col min="25" max="26" width="8.796875" style="3" bestFit="1" customWidth="1"/>
     <col min="27" max="16384" width="8.59765625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="F1" s="41" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="F1" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="K1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="K1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
       <c r="R1" s="1" t="s">
         <v>25</v>
       </c>
@@ -5946,6 +5945,10 @@
       </c>
       <c r="P2" s="9" t="s">
         <v>20</v>
+      </c>
+      <c r="Y2" s="3" cm="1">
+        <f t="array" ref="Y2:Y13">800-_xlfn.BYROW(S19:U30,_xlfn.LAMBDA(_xlpm.r,SUM(_xlpm.r)))</f>
+        <v>680</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
@@ -5980,6 +5983,9 @@
       <c r="N3" s="33"/>
       <c r="O3" s="14"/>
       <c r="P3" s="15"/>
+      <c r="Y3" s="3">
+        <v>444</v>
+      </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -6026,6 +6032,9 @@
         <f t="array" ref="V4:V6">_xlfn.BYROW(R4:T6,_xlfn.LAMBDA(_xlpm.r,SUM(_xlpm.r)))</f>
         <v>6</v>
       </c>
+      <c r="Y4" s="3">
+        <v>514</v>
+      </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -6076,6 +6085,9 @@
       </c>
       <c r="V5" s="3">
         <v>15</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>800</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
@@ -6122,6 +6134,9 @@
       <c r="V6" s="3">
         <v>24</v>
       </c>
+      <c r="Y6" s="3">
+        <v>800</v>
+      </c>
       <c r="AE6" s="36" cm="1">
         <f t="array" ref="AE6:AE17">D3:D14</f>
         <v>120</v>
@@ -6180,6 +6195,9 @@
       <c r="R7" s="38"/>
       <c r="S7" s="38"/>
       <c r="T7" s="38"/>
+      <c r="Y7" s="3">
+        <v>800</v>
+      </c>
       <c r="AE7" s="3">
         <v>356</v>
       </c>
@@ -6220,6 +6238,9 @@
       <c r="P8" s="34">
         <v>258</v>
       </c>
+      <c r="Y8" s="3">
+        <v>800</v>
+      </c>
       <c r="AE8" s="3">
         <v>312</v>
       </c>
@@ -6260,6 +6281,9 @@
       <c r="P9" s="34">
         <v>369</v>
       </c>
+      <c r="Y9" s="3">
+        <v>800</v>
+      </c>
       <c r="AE9" s="3">
         <v>437</v>
       </c>
@@ -6300,6 +6324,9 @@
       <c r="P10" s="34">
         <v>418</v>
       </c>
+      <c r="Y10" s="3">
+        <v>800</v>
+      </c>
       <c r="AE10" s="3">
         <v>374</v>
       </c>
@@ -6340,6 +6367,9 @@
       <c r="P11" s="34">
         <v>308</v>
       </c>
+      <c r="Y11" s="3">
+        <v>800</v>
+      </c>
       <c r="AE11" s="3">
         <v>258</v>
       </c>
@@ -6381,6 +6411,9 @@
       <c r="P12" s="34">
         <v>410</v>
       </c>
+      <c r="Y12" s="3">
+        <v>800</v>
+      </c>
       <c r="AE12" s="3">
         <v>369</v>
       </c>
@@ -6429,6 +6462,9 @@
       </c>
       <c r="P13" s="15" t="s">
         <v>21</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>800</v>
       </c>
       <c r="AE13" s="3">
         <v>418</v>
@@ -6547,6 +6583,21 @@
       <c r="G17" s="20"/>
       <c r="L17" s="27"/>
       <c r="O17" s="20"/>
+      <c r="S17">
+        <v>600</v>
+      </c>
+      <c r="T17">
+        <v>50</v>
+      </c>
+      <c r="U17">
+        <v>112</v>
+      </c>
+      <c r="V17">
+        <v>800</v>
+      </c>
+      <c r="W17">
+        <v>1800</v>
+      </c>
       <c r="AE17" s="3">
         <v>50</v>
       </c>
@@ -7742,8 +7793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9A81A7-D6B7-40E5-911B-C548F7BC223F}">
   <dimension ref="B1:X74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -7764,24 +7815,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="F1" s="41" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="F1" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="K1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="K1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
       <c r="R1" s="1" t="s">
         <v>25</v>
       </c>
@@ -7821,7 +7872,7 @@
       <c r="P2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="43" t="s">
+      <c r="R2" s="41" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>